<commit_message>
Inclusao dos graficos nas abas das planilhas
</commit_message>
<xml_diff>
--- a/documentos/dataset_detalhes.xlsx
+++ b/documentos/dataset_detalhes.xlsx
@@ -7,19 +7,21 @@
     <workbookView xWindow="0" yWindow="75" windowWidth="38355" windowHeight="12600"/>
   </bookViews>
   <sheets>
-    <sheet name="Plan1" sheetId="1" r:id="rId1"/>
-    <sheet name="Plan2" sheetId="2" r:id="rId2"/>
-    <sheet name="Plan3" sheetId="3" r:id="rId3"/>
+    <sheet name="Questionario" sheetId="1" r:id="rId1"/>
+    <sheet name="1.Genero" sheetId="2" r:id="rId2"/>
+    <sheet name="1.Idade" sheetId="3" r:id="rId3"/>
+    <sheet name="1.Sit_conjugal" sheetId="4" r:id="rId4"/>
+    <sheet name="1.Sit_emprego" sheetId="5" r:id="rId5"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Plan1!$H$1:$J$53</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Questionario!$A$1:$K$69</definedName>
   </definedNames>
   <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="430" uniqueCount="143">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="446" uniqueCount="155">
   <si>
     <t>Sequencia</t>
   </si>
@@ -423,9 +425,6 @@
     <t>verificar multi opcao</t>
   </si>
   <si>
-    <t>Dados basicos e pessoais</t>
-  </si>
-  <si>
     <t>Instituicao de Ensino x Pandemia</t>
   </si>
   <si>
@@ -448,6 +447,45 @@
   </si>
   <si>
     <t>assunto</t>
+  </si>
+  <si>
+    <t>1. Dados basicos e pessoais</t>
+  </si>
+  <si>
+    <t>Feito_Analise_Grafico</t>
+  </si>
+  <si>
+    <t>Dados Pessoais</t>
+  </si>
+  <si>
+    <t>Genero</t>
+  </si>
+  <si>
+    <t xml:space="preserve">                  Var1 Freq</t>
+  </si>
+  <si>
+    <t>1               Feminino   24</t>
+  </si>
+  <si>
+    <t>2              Homem gay    1</t>
+  </si>
+  <si>
+    <t>3              Masculino   25</t>
+  </si>
+  <si>
+    <t>4 Transgênero/Transexual    2</t>
+  </si>
+  <si>
+    <t>Maioria Feminino e Masculino</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dados Pessoais </t>
+  </si>
+  <si>
+    <t>Idade (Faixa Etaria)</t>
+  </si>
+  <si>
+    <t>Maioria (17 a 24 anos) 35%</t>
   </si>
 </sst>
 </file>
@@ -544,7 +582,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="14" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
@@ -591,6 +629,7 @@
     <xf numFmtId="14" fontId="2" fillId="8" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="9" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -599,6 +638,92 @@
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>266700</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>173139</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>19782</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Imagem 1" descr="grafico_genero.png"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3295650" y="304800"/>
+          <a:ext cx="12098439" cy="5239482"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>571500</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>77889</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>134082</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Imagem 2" descr="grafico_faixa_etaria2.png"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1571625" y="609600"/>
+          <a:ext cx="12098439" cy="5239482"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -890,7 +1015,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J6" sqref="J6"/>
+      <selection pane="bottomLeft" activeCell="K3" sqref="K3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -903,6 +1028,7 @@
     <col min="8" max="8" width="16.85546875" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="15" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="30.7109375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="20.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:52">
@@ -931,7 +1057,10 @@
         <v>17</v>
       </c>
       <c r="J1" t="s">
-        <v>142</v>
+        <v>141</v>
+      </c>
+      <c r="K1" t="s">
+        <v>143</v>
       </c>
     </row>
     <row r="2" spans="1:52">
@@ -955,6 +1084,7 @@
       </c>
       <c r="I2" s="6"/>
       <c r="J2" s="6"/>
+      <c r="K2" s="6"/>
     </row>
     <row r="3" spans="1:52">
       <c r="A3" s="7" t="s">
@@ -981,7 +1111,10 @@
       </c>
       <c r="I3" s="9"/>
       <c r="J3" s="9" t="s">
-        <v>134</v>
+        <v>142</v>
+      </c>
+      <c r="K3" s="9" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="4" spans="1:52">
@@ -1009,7 +1142,10 @@
       </c>
       <c r="I4" s="9"/>
       <c r="J4" s="9" t="s">
-        <v>134</v>
+        <v>142</v>
+      </c>
+      <c r="K4" s="9" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="5" spans="1:52">
@@ -1037,7 +1173,7 @@
       </c>
       <c r="I5" s="9"/>
       <c r="J5" s="9" t="s">
-        <v>134</v>
+        <v>142</v>
       </c>
     </row>
     <row r="6" spans="1:52">
@@ -1065,7 +1201,7 @@
       </c>
       <c r="I6" s="9"/>
       <c r="J6" s="9" t="s">
-        <v>134</v>
+        <v>142</v>
       </c>
     </row>
     <row r="7" spans="1:52">
@@ -1093,7 +1229,7 @@
       </c>
       <c r="I7" s="9"/>
       <c r="J7" s="9" t="s">
-        <v>134</v>
+        <v>142</v>
       </c>
     </row>
     <row r="8" spans="1:52">
@@ -1121,7 +1257,10 @@
       </c>
       <c r="I8" s="9"/>
       <c r="J8" s="9" t="s">
-        <v>134</v>
+        <v>142</v>
+      </c>
+      <c r="K8" s="9" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="9" spans="1:52">
@@ -1149,7 +1288,7 @@
       </c>
       <c r="I9" s="9"/>
       <c r="J9" s="9" t="s">
-        <v>134</v>
+        <v>142</v>
       </c>
     </row>
     <row r="10" spans="1:52">
@@ -1177,7 +1316,10 @@
       </c>
       <c r="I10" s="9"/>
       <c r="J10" s="9" t="s">
-        <v>134</v>
+        <v>142</v>
+      </c>
+      <c r="K10" s="9" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="11" spans="1:52">
@@ -1205,7 +1347,7 @@
       </c>
       <c r="I11" s="9"/>
       <c r="J11" s="9" t="s">
-        <v>134</v>
+        <v>142</v>
       </c>
     </row>
     <row r="12" spans="1:52">
@@ -1233,7 +1375,7 @@
       </c>
       <c r="I12" s="9"/>
       <c r="J12" s="9" t="s">
-        <v>134</v>
+        <v>142</v>
       </c>
     </row>
     <row r="13" spans="1:52">
@@ -1261,7 +1403,7 @@
       </c>
       <c r="I13" s="9"/>
       <c r="J13" s="9" t="s">
-        <v>134</v>
+        <v>142</v>
       </c>
     </row>
     <row r="14" spans="1:52">
@@ -1289,7 +1431,7 @@
       </c>
       <c r="I14" s="26"/>
       <c r="J14" s="26" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="15" spans="1:52">
@@ -1317,7 +1459,7 @@
       </c>
       <c r="I15" s="26"/>
       <c r="J15" s="26" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="16" spans="1:52">
@@ -1347,7 +1489,7 @@
         <v>132</v>
       </c>
       <c r="J16" s="26" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="K16" s="1"/>
       <c r="L16" s="1"/>
@@ -1417,7 +1559,7 @@
       </c>
       <c r="I17" s="26"/>
       <c r="J17" s="26" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="18" spans="1:10">
@@ -1445,7 +1587,7 @@
       </c>
       <c r="I18" s="9"/>
       <c r="J18" s="9" t="s">
-        <v>134</v>
+        <v>142</v>
       </c>
     </row>
     <row r="19" spans="1:10">
@@ -1473,7 +1615,7 @@
       </c>
       <c r="I19" s="9"/>
       <c r="J19" s="9" t="s">
-        <v>134</v>
+        <v>142</v>
       </c>
     </row>
     <row r="20" spans="1:10">
@@ -1501,7 +1643,7 @@
       </c>
       <c r="I20" s="9"/>
       <c r="J20" s="9" t="s">
-        <v>134</v>
+        <v>142</v>
       </c>
     </row>
     <row r="21" spans="1:10">
@@ -1529,7 +1671,7 @@
       </c>
       <c r="I21" s="23"/>
       <c r="J21" s="23" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="22" spans="1:10">
@@ -1557,7 +1699,7 @@
       </c>
       <c r="I22" s="23"/>
       <c r="J22" s="23" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="23" spans="1:10">
@@ -1585,7 +1727,7 @@
       </c>
       <c r="I23" s="23"/>
       <c r="J23" s="23" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="24" spans="1:10">
@@ -1613,7 +1755,7 @@
       </c>
       <c r="I24" s="23"/>
       <c r="J24" s="23" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="25" spans="1:10">
@@ -1641,7 +1783,7 @@
       </c>
       <c r="I25" s="23"/>
       <c r="J25" s="23" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="26" spans="1:10">
@@ -1669,7 +1811,7 @@
       </c>
       <c r="I26" s="14"/>
       <c r="J26" s="14" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="27" spans="1:10">
@@ -1697,7 +1839,7 @@
       </c>
       <c r="I27" s="17"/>
       <c r="J27" s="17" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="28" spans="1:10">
@@ -1725,7 +1867,7 @@
       </c>
       <c r="I28" s="23"/>
       <c r="J28" s="23" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="29" spans="1:10">
@@ -1755,7 +1897,7 @@
         <v>132</v>
       </c>
       <c r="J29" s="23" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="30" spans="1:10">
@@ -1783,7 +1925,7 @@
       </c>
       <c r="I30" s="14"/>
       <c r="J30" s="14" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="31" spans="1:10">
@@ -1811,7 +1953,7 @@
       </c>
       <c r="I31" s="14"/>
       <c r="J31" s="14" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="32" spans="1:10">
@@ -1839,7 +1981,7 @@
       </c>
       <c r="I32" s="26"/>
       <c r="J32" s="26" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="33" spans="1:10">
@@ -1867,7 +2009,7 @@
       </c>
       <c r="I33" s="14"/>
       <c r="J33" s="14" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="34" spans="1:10">
@@ -1895,7 +2037,7 @@
       </c>
       <c r="I34" s="14"/>
       <c r="J34" s="14" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="35" spans="1:10">
@@ -1923,7 +2065,7 @@
       </c>
       <c r="I35" s="14"/>
       <c r="J35" s="14" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="36" spans="1:10">
@@ -1951,7 +2093,7 @@
       </c>
       <c r="I36" s="26"/>
       <c r="J36" s="26" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="37" spans="1:10">
@@ -1979,7 +2121,7 @@
       </c>
       <c r="I37" s="26"/>
       <c r="J37" s="26" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="38" spans="1:10">
@@ -2007,7 +2149,7 @@
       </c>
       <c r="I38" s="23"/>
       <c r="J38" s="23" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="39" spans="1:10">
@@ -2037,7 +2179,7 @@
         <v>132</v>
       </c>
       <c r="J39" s="14" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="40" spans="1:10">
@@ -2065,7 +2207,7 @@
       </c>
       <c r="I40" s="20"/>
       <c r="J40" s="20" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="41" spans="1:10">
@@ -2093,7 +2235,7 @@
       </c>
       <c r="I41" s="20"/>
       <c r="J41" s="20" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="42" spans="1:10">
@@ -2121,7 +2263,7 @@
       </c>
       <c r="I42" s="20"/>
       <c r="J42" s="20" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="43" spans="1:10">
@@ -2149,7 +2291,7 @@
       </c>
       <c r="I43" s="20"/>
       <c r="J43" s="20" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="44" spans="1:10">
@@ -2177,7 +2319,7 @@
       </c>
       <c r="I44" s="20"/>
       <c r="J44" s="20" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="45" spans="1:10">
@@ -2207,7 +2349,7 @@
         <v>132</v>
       </c>
       <c r="J45" s="20" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="46" spans="1:10">
@@ -2235,7 +2377,7 @@
       </c>
       <c r="I46" s="26"/>
       <c r="J46" s="26" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="47" spans="1:10">
@@ -2265,7 +2407,7 @@
         <v>132</v>
       </c>
       <c r="J47" s="26" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="48" spans="1:10">
@@ -2295,7 +2437,7 @@
         <v>132</v>
       </c>
       <c r="J48" s="26" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="49" spans="1:10">
@@ -2325,7 +2467,7 @@
         <v>132</v>
       </c>
       <c r="J49" s="26" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="50" spans="1:10">
@@ -2353,7 +2495,7 @@
       </c>
       <c r="I50" s="23"/>
       <c r="J50" s="23" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="51" spans="1:10">
@@ -2381,7 +2523,7 @@
       </c>
       <c r="I51" s="23"/>
       <c r="J51" s="23" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="52" spans="1:10">
@@ -2409,7 +2551,7 @@
       </c>
       <c r="I52" s="23"/>
       <c r="J52" s="23" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="53" spans="1:10">
@@ -2439,7 +2581,7 @@
         <v>132</v>
       </c>
       <c r="J53" s="11" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="54" spans="1:10">
@@ -2500,16 +2642,117 @@
       <c r="A69" s="1"/>
     </row>
   </sheetData>
-  <autoFilter ref="H1:J53"/>
+  <autoFilter ref="A1:K69"/>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:C7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="27.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3">
+      <c r="A1" t="s">
+        <v>144</v>
+      </c>
+      <c r="B1" t="s">
+        <v>145</v>
+      </c>
+      <c r="C1" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4" t="s">
+        <v>147</v>
+      </c>
+      <c r="B4" s="30">
+        <v>0.46</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="A5" t="s">
+        <v>148</v>
+      </c>
+      <c r="B5" s="30">
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
+      <c r="A6" t="s">
+        <v>149</v>
+      </c>
+      <c r="B6" s="30">
+        <v>0.48</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3">
+      <c r="A7" t="s">
+        <v>150</v>
+      </c>
+      <c r="B7" s="30">
+        <v>0.04</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:C1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="15" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="24.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3">
+      <c r="A1" t="s">
+        <v>152</v>
+      </c>
+      <c r="B1" t="s">
+        <v>153</v>
+      </c>
+      <c r="C1" t="s">
+        <v>154</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I34" sqref="I34"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData/>
@@ -2517,11 +2760,13 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G35" sqref="G35"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData/>

</xml_diff>

<commit_message>
Atualizando codigo, planilha e um diretorio com todos os graficos gerados.
</commit_message>
<xml_diff>
--- a/documentos/dataset_detalhes.xlsx
+++ b/documentos/dataset_detalhes.xlsx
@@ -12,6 +12,8 @@
     <sheet name="1.Idade" sheetId="3" r:id="rId3"/>
     <sheet name="1.Sit_conjugal" sheetId="4" r:id="rId4"/>
     <sheet name="1.Sit_emprego" sheetId="5" r:id="rId5"/>
+    <sheet name="1.Estado_resid" sheetId="6" r:id="rId6"/>
+    <sheet name="1.Inst_ensino" sheetId="7" r:id="rId7"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Questionario!$A$1:$K$69</definedName>
@@ -21,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="446" uniqueCount="155">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="460" uniqueCount="165">
   <si>
     <t>Sequencia</t>
   </si>
@@ -486,6 +488,36 @@
   </si>
   <si>
     <t>Maioria (17 a 24 anos) 35%</t>
+  </si>
+  <si>
+    <t>Obs</t>
+  </si>
+  <si>
+    <t>Maioria 17 a 24 anos</t>
+  </si>
+  <si>
+    <t>Maioria Masculino e Feminino</t>
+  </si>
+  <si>
+    <t>Maioria UNESP Bauru</t>
+  </si>
+  <si>
+    <t>1.Situacao Conjugal</t>
+  </si>
+  <si>
+    <t>1.Situacao Emprego</t>
+  </si>
+  <si>
+    <t>1.Instituicao de Ensino</t>
+  </si>
+  <si>
+    <t>UNESP Bauru</t>
+  </si>
+  <si>
+    <t>Demais</t>
+  </si>
+  <si>
+    <t>Maioria Solteiro</t>
   </si>
 </sst>
 </file>
@@ -582,7 +614,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="14" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
@@ -630,6 +662,7 @@
     <xf numFmtId="0" fontId="2" fillId="9" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -714,6 +747,92 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="1571625" y="609600"/>
+          <a:ext cx="12098439" cy="5239482"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>390525</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>85725</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>363480</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>181707</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Imagem 1" descr="1_situacao_conjugal.png"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1362075" y="657225"/>
+          <a:ext cx="10955280" cy="5239482"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>514350</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>104775</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>420789</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>10257</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Imagem 1" descr="grafico_inst_ensino.png"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2705100" y="485775"/>
           <a:ext cx="12098439" cy="5239482"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -1015,7 +1134,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K11" sqref="K11"/>
+      <selection pane="bottomLeft" activeCell="K6" sqref="K6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1029,6 +1148,7 @@
     <col min="9" max="9" width="15" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="30.7109375" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="20.7109375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="28.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:52">
@@ -1062,6 +1182,9 @@
       <c r="K1" t="s">
         <v>143</v>
       </c>
+      <c r="L1" t="s">
+        <v>155</v>
+      </c>
     </row>
     <row r="2" spans="1:52">
       <c r="A2" s="4" t="s">
@@ -1085,6 +1208,7 @@
       <c r="I2" s="6"/>
       <c r="J2" s="6"/>
       <c r="K2" s="6"/>
+      <c r="L2" s="6"/>
     </row>
     <row r="3" spans="1:52">
       <c r="A3" s="7" t="s">
@@ -1116,6 +1240,9 @@
       <c r="K3" s="9" t="s">
         <v>9</v>
       </c>
+      <c r="L3" s="9" t="s">
+        <v>156</v>
+      </c>
     </row>
     <row r="4" spans="1:52">
       <c r="A4" s="7" t="s">
@@ -1147,6 +1274,9 @@
       <c r="K4" s="9" t="s">
         <v>9</v>
       </c>
+      <c r="L4" s="9" t="s">
+        <v>157</v>
+      </c>
     </row>
     <row r="5" spans="1:52">
       <c r="A5" s="7" t="s">
@@ -1175,6 +1305,12 @@
       <c r="J5" s="9" t="s">
         <v>142</v>
       </c>
+      <c r="K5" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="L5" s="9" t="s">
+        <v>164</v>
+      </c>
     </row>
     <row r="6" spans="1:52">
       <c r="A6" s="7" t="s">
@@ -1261,6 +1397,9 @@
       </c>
       <c r="K8" s="9" t="s">
         <v>9</v>
+      </c>
+      <c r="L8" s="9" t="s">
+        <v>158</v>
       </c>
     </row>
     <row r="9" spans="1:52">
@@ -2748,11 +2887,64 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:B1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="V12" sqref="V12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" t="s">
+        <v>144</v>
+      </c>
+      <c r="B1" t="s">
+        <v>159</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:B1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" t="s">
+        <v>144</v>
+      </c>
+      <c r="B1" t="s">
+        <v>160</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I34" sqref="I34"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData/>
@@ -2760,16 +2952,51 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+  <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G35" sqref="G35"/>
+      <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="14.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3">
+      <c r="A1" t="s">
+        <v>144</v>
+      </c>
+      <c r="B1" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3" t="s">
+        <v>162</v>
+      </c>
+      <c r="B3" s="31">
+        <v>40</v>
+      </c>
+      <c r="C3" s="30">
+        <v>0.77</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4" t="s">
+        <v>163</v>
+      </c>
+      <c r="B4" s="31">
+        <v>12</v>
+      </c>
+      <c r="C4" s="30">
+        <v>0.23</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Codigo e demais graficos de dados pessoais.
</commit_message>
<xml_diff>
--- a/documentos/dataset_detalhes.xlsx
+++ b/documentos/dataset_detalhes.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="464" uniqueCount="167">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="467" uniqueCount="169">
   <si>
     <t>Sequencia</t>
   </si>
@@ -524,6 +524,12 @@
   </si>
   <si>
     <t>Maioria SP</t>
+  </si>
+  <si>
+    <t>Maioria Graduacao (21) e depois Doutorado(15) e Mestrado (13)</t>
+  </si>
+  <si>
+    <t>Maioria PPGMit (psicologia duplicado)</t>
   </si>
 </sst>
 </file>
@@ -1145,11 +1151,12 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="1"/>
   <dimension ref="A1:AZ69"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A10" sqref="A10"/>
+      <selection pane="bottomLeft" activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1201,7 +1208,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="2" spans="1:52">
+    <row r="2" spans="1:52" hidden="1">
       <c r="A2" s="4" t="s">
         <v>67</v>
       </c>
@@ -1456,6 +1463,12 @@
       <c r="J9" s="9" t="s">
         <v>142</v>
       </c>
+      <c r="K9" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="L9" s="9" t="s">
+        <v>168</v>
+      </c>
     </row>
     <row r="10" spans="1:52">
       <c r="A10" s="7" t="s">
@@ -1487,6 +1500,9 @@
       <c r="K10" s="9" t="s">
         <v>9</v>
       </c>
+      <c r="L10" s="9" t="s">
+        <v>167</v>
+      </c>
     </row>
     <row r="11" spans="1:52">
       <c r="A11" s="7" t="s">
@@ -1572,7 +1588,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="14" spans="1:52">
+    <row r="14" spans="1:52" hidden="1">
       <c r="A14" s="24" t="s">
         <v>79</v>
       </c>
@@ -1600,7 +1616,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="15" spans="1:52">
+    <row r="15" spans="1:52" hidden="1">
       <c r="A15" s="24" t="s">
         <v>80</v>
       </c>
@@ -1628,7 +1644,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="16" spans="1:52">
+    <row r="16" spans="1:52" hidden="1">
       <c r="A16" s="24" t="s">
         <v>81</v>
       </c>
@@ -1700,7 +1716,7 @@
       <c r="AY16" s="1"/>
       <c r="AZ16" s="1"/>
     </row>
-    <row r="17" spans="1:10">
+    <row r="17" spans="1:10" hidden="1">
       <c r="A17" s="24" t="s">
         <v>82</v>
       </c>
@@ -1812,7 +1828,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="21" spans="1:10">
+    <row r="21" spans="1:10" hidden="1">
       <c r="A21" s="21" t="s">
         <v>86</v>
       </c>
@@ -1840,7 +1856,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="22" spans="1:10">
+    <row r="22" spans="1:10" hidden="1">
       <c r="A22" s="21" t="s">
         <v>87</v>
       </c>
@@ -1868,7 +1884,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="23" spans="1:10">
+    <row r="23" spans="1:10" hidden="1">
       <c r="A23" s="21" t="s">
         <v>88</v>
       </c>
@@ -1896,7 +1912,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="24" spans="1:10">
+    <row r="24" spans="1:10" hidden="1">
       <c r="A24" s="21" t="s">
         <v>89</v>
       </c>
@@ -1924,7 +1940,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="25" spans="1:10">
+    <row r="25" spans="1:10" hidden="1">
       <c r="A25" s="21" t="s">
         <v>90</v>
       </c>
@@ -1952,7 +1968,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="26" spans="1:10">
+    <row r="26" spans="1:10" hidden="1">
       <c r="A26" s="12" t="s">
         <v>91</v>
       </c>
@@ -1980,7 +1996,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="27" spans="1:10">
+    <row r="27" spans="1:10" hidden="1">
       <c r="A27" s="15" t="s">
         <v>92</v>
       </c>
@@ -2008,7 +2024,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="28" spans="1:10">
+    <row r="28" spans="1:10" hidden="1">
       <c r="A28" s="21" t="s">
         <v>93</v>
       </c>
@@ -2036,7 +2052,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="29" spans="1:10">
+    <row r="29" spans="1:10" hidden="1">
       <c r="A29" s="21" t="s">
         <v>94</v>
       </c>
@@ -2066,7 +2082,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="30" spans="1:10">
+    <row r="30" spans="1:10" hidden="1">
       <c r="A30" s="12" t="s">
         <v>95</v>
       </c>
@@ -2094,7 +2110,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="31" spans="1:10">
+    <row r="31" spans="1:10" hidden="1">
       <c r="A31" s="12" t="s">
         <v>96</v>
       </c>
@@ -2122,7 +2138,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="32" spans="1:10">
+    <row r="32" spans="1:10" hidden="1">
       <c r="A32" s="24" t="s">
         <v>97</v>
       </c>
@@ -2150,7 +2166,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="33" spans="1:10">
+    <row r="33" spans="1:10" hidden="1">
       <c r="A33" s="12" t="s">
         <v>98</v>
       </c>
@@ -2178,7 +2194,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="34" spans="1:10">
+    <row r="34" spans="1:10" hidden="1">
       <c r="A34" s="12" t="s">
         <v>99</v>
       </c>
@@ -2206,7 +2222,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="35" spans="1:10">
+    <row r="35" spans="1:10" hidden="1">
       <c r="A35" s="12" t="s">
         <v>100</v>
       </c>
@@ -2234,7 +2250,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="36" spans="1:10">
+    <row r="36" spans="1:10" hidden="1">
       <c r="A36" s="24" t="s">
         <v>101</v>
       </c>
@@ -2262,7 +2278,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="37" spans="1:10">
+    <row r="37" spans="1:10" hidden="1">
       <c r="A37" s="24" t="s">
         <v>102</v>
       </c>
@@ -2290,7 +2306,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="38" spans="1:10">
+    <row r="38" spans="1:10" hidden="1">
       <c r="A38" s="21" t="s">
         <v>103</v>
       </c>
@@ -2318,7 +2334,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="39" spans="1:10">
+    <row r="39" spans="1:10" hidden="1">
       <c r="A39" s="12" t="s">
         <v>104</v>
       </c>
@@ -2348,7 +2364,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="40" spans="1:10">
+    <row r="40" spans="1:10" hidden="1">
       <c r="A40" s="18" t="s">
         <v>105</v>
       </c>
@@ -2376,7 +2392,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="41" spans="1:10">
+    <row r="41" spans="1:10" hidden="1">
       <c r="A41" s="18" t="s">
         <v>106</v>
       </c>
@@ -2404,7 +2420,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="42" spans="1:10">
+    <row r="42" spans="1:10" hidden="1">
       <c r="A42" s="18" t="s">
         <v>107</v>
       </c>
@@ -2432,7 +2448,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="43" spans="1:10">
+    <row r="43" spans="1:10" hidden="1">
       <c r="A43" s="18" t="s">
         <v>108</v>
       </c>
@@ -2460,7 +2476,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="44" spans="1:10">
+    <row r="44" spans="1:10" hidden="1">
       <c r="A44" s="18" t="s">
         <v>109</v>
       </c>
@@ -2488,7 +2504,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="45" spans="1:10">
+    <row r="45" spans="1:10" hidden="1">
       <c r="A45" s="18" t="s">
         <v>110</v>
       </c>
@@ -2518,7 +2534,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="46" spans="1:10">
+    <row r="46" spans="1:10" hidden="1">
       <c r="A46" s="24" t="s">
         <v>111</v>
       </c>
@@ -2546,7 +2562,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="47" spans="1:10">
+    <row r="47" spans="1:10" hidden="1">
       <c r="A47" s="24" t="s">
         <v>112</v>
       </c>
@@ -2576,7 +2592,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="48" spans="1:10">
+    <row r="48" spans="1:10" hidden="1">
       <c r="A48" s="24" t="s">
         <v>113</v>
       </c>
@@ -2606,7 +2622,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="49" spans="1:10">
+    <row r="49" spans="1:10" hidden="1">
       <c r="A49" s="24" t="s">
         <v>114</v>
       </c>
@@ -2636,7 +2652,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="50" spans="1:10">
+    <row r="50" spans="1:10" hidden="1">
       <c r="A50" s="21" t="s">
         <v>115</v>
       </c>
@@ -2664,7 +2680,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="51" spans="1:10">
+    <row r="51" spans="1:10" hidden="1">
       <c r="A51" s="21" t="s">
         <v>116</v>
       </c>
@@ -2692,7 +2708,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="52" spans="1:10">
+    <row r="52" spans="1:10" hidden="1">
       <c r="A52" s="21" t="s">
         <v>117</v>
       </c>
@@ -2720,7 +2736,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="53" spans="1:10">
+    <row r="53" spans="1:10" hidden="1">
       <c r="A53" s="3" t="s">
         <v>118</v>
       </c>
@@ -2750,7 +2766,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="54" spans="1:10">
+    <row r="54" spans="1:10" hidden="1">
       <c r="A54" s="28"/>
       <c r="B54" s="29"/>
       <c r="C54" s="29"/>
@@ -2762,53 +2778,59 @@
       <c r="I54" s="29"/>
       <c r="J54" s="29"/>
     </row>
-    <row r="55" spans="1:10">
+    <row r="55" spans="1:10" hidden="1">
       <c r="A55" s="1"/>
     </row>
-    <row r="56" spans="1:10">
+    <row r="56" spans="1:10" hidden="1">
       <c r="A56" s="1"/>
     </row>
-    <row r="57" spans="1:10">
+    <row r="57" spans="1:10" hidden="1">
       <c r="A57" s="1"/>
     </row>
-    <row r="58" spans="1:10">
+    <row r="58" spans="1:10" hidden="1">
       <c r="A58" s="1"/>
     </row>
-    <row r="59" spans="1:10">
+    <row r="59" spans="1:10" hidden="1">
       <c r="A59" s="1"/>
     </row>
-    <row r="60" spans="1:10">
+    <row r="60" spans="1:10" hidden="1">
       <c r="A60" s="1"/>
     </row>
-    <row r="61" spans="1:10">
+    <row r="61" spans="1:10" hidden="1">
       <c r="A61" s="1"/>
     </row>
-    <row r="62" spans="1:10">
+    <row r="62" spans="1:10" hidden="1">
       <c r="A62" s="1"/>
     </row>
-    <row r="63" spans="1:10">
+    <row r="63" spans="1:10" hidden="1">
       <c r="A63" s="1"/>
     </row>
-    <row r="64" spans="1:10">
+    <row r="64" spans="1:10" hidden="1">
       <c r="A64" s="1"/>
     </row>
-    <row r="65" spans="1:1">
+    <row r="65" spans="1:1" hidden="1">
       <c r="A65" s="1"/>
     </row>
-    <row r="66" spans="1:1">
+    <row r="66" spans="1:1" hidden="1">
       <c r="A66" s="1"/>
     </row>
-    <row r="67" spans="1:1">
+    <row r="67" spans="1:1" hidden="1">
       <c r="A67" s="1"/>
     </row>
-    <row r="68" spans="1:1">
+    <row r="68" spans="1:1" hidden="1">
       <c r="A68" s="1"/>
     </row>
-    <row r="69" spans="1:1">
+    <row r="69" spans="1:1" hidden="1">
       <c r="A69" s="1"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:K69"/>
+  <autoFilter ref="A1:K69">
+    <filterColumn colId="9">
+      <filters>
+        <filter val="1. Dados basicos e pessoais"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
Codigo e finalizado graficos de dados pessoais
</commit_message>
<xml_diff>
--- a/documentos/dataset_detalhes.xlsx
+++ b/documentos/dataset_detalhes.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="467" uniqueCount="169">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="479" uniqueCount="176">
   <si>
     <t>Sequencia</t>
   </si>
@@ -530,6 +530,27 @@
   </si>
   <si>
     <t>Maioria PPGMit (psicologia duplicado)</t>
+  </si>
+  <si>
+    <t>Data de inicio do curso, sem necessida de grafico</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sim </t>
+  </si>
+  <si>
+    <t>Maioria Publica</t>
+  </si>
+  <si>
+    <t>Maioria de não é um estudante nativo</t>
+  </si>
+  <si>
+    <t>maioria mora na mesma cidade do campus</t>
+  </si>
+  <si>
+    <t>Maioria tem moradia permanente e estavel</t>
+  </si>
+  <si>
+    <t>Maioria mora com familia</t>
   </si>
 </sst>
 </file>
@@ -1156,7 +1177,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B11" sqref="B11"/>
+      <selection pane="bottomLeft" activeCell="A20" sqref="A20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1531,6 +1552,12 @@
       <c r="J11" s="9" t="s">
         <v>142</v>
       </c>
+      <c r="K11" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="L11" s="9" t="s">
+        <v>169</v>
+      </c>
     </row>
     <row r="12" spans="1:52">
       <c r="A12" s="7" t="s">
@@ -1559,6 +1586,12 @@
       <c r="J12" s="9" t="s">
         <v>142</v>
       </c>
+      <c r="K12" s="9" t="s">
+        <v>170</v>
+      </c>
+      <c r="L12" s="9" t="s">
+        <v>171</v>
+      </c>
     </row>
     <row r="13" spans="1:52">
       <c r="A13" s="7" t="s">
@@ -1586,6 +1619,12 @@
       <c r="I13" s="9"/>
       <c r="J13" s="9" t="s">
         <v>142</v>
+      </c>
+      <c r="K13" s="9" t="s">
+        <v>170</v>
+      </c>
+      <c r="L13" s="9" t="s">
+        <v>172</v>
       </c>
     </row>
     <row r="14" spans="1:52" hidden="1">
@@ -1716,7 +1755,7 @@
       <c r="AY16" s="1"/>
       <c r="AZ16" s="1"/>
     </row>
-    <row r="17" spans="1:10" hidden="1">
+    <row r="17" spans="1:12" hidden="1">
       <c r="A17" s="24" t="s">
         <v>82</v>
       </c>
@@ -1744,7 +1783,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="18" spans="1:10">
+    <row r="18" spans="1:12">
       <c r="A18" s="7" t="s">
         <v>83</v>
       </c>
@@ -1771,8 +1810,14 @@
       <c r="J18" s="9" t="s">
         <v>142</v>
       </c>
-    </row>
-    <row r="19" spans="1:10">
+      <c r="K18" s="9" t="s">
+        <v>170</v>
+      </c>
+      <c r="L18" s="9" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12">
       <c r="A19" s="7" t="s">
         <v>84</v>
       </c>
@@ -1799,8 +1844,14 @@
       <c r="J19" s="9" t="s">
         <v>142</v>
       </c>
-    </row>
-    <row r="20" spans="1:10">
+      <c r="K19" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="L19" s="9" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12">
       <c r="A20" s="7" t="s">
         <v>85</v>
       </c>
@@ -1827,8 +1878,14 @@
       <c r="J20" s="9" t="s">
         <v>142</v>
       </c>
-    </row>
-    <row r="21" spans="1:10" hidden="1">
+      <c r="K20" s="9" t="s">
+        <v>170</v>
+      </c>
+      <c r="L20" s="9" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" hidden="1">
       <c r="A21" s="21" t="s">
         <v>86</v>
       </c>
@@ -1856,7 +1913,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="22" spans="1:10" hidden="1">
+    <row r="22" spans="1:12" hidden="1">
       <c r="A22" s="21" t="s">
         <v>87</v>
       </c>
@@ -1884,7 +1941,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="23" spans="1:10" hidden="1">
+    <row r="23" spans="1:12" hidden="1">
       <c r="A23" s="21" t="s">
         <v>88</v>
       </c>
@@ -1912,7 +1969,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="24" spans="1:10" hidden="1">
+    <row r="24" spans="1:12" hidden="1">
       <c r="A24" s="21" t="s">
         <v>89</v>
       </c>
@@ -1940,7 +1997,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="25" spans="1:10" hidden="1">
+    <row r="25" spans="1:12" hidden="1">
       <c r="A25" s="21" t="s">
         <v>90</v>
       </c>
@@ -1968,7 +2025,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="26" spans="1:10" hidden="1">
+    <row r="26" spans="1:12" hidden="1">
       <c r="A26" s="12" t="s">
         <v>91</v>
       </c>
@@ -1996,7 +2053,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="27" spans="1:10" hidden="1">
+    <row r="27" spans="1:12" hidden="1">
       <c r="A27" s="15" t="s">
         <v>92</v>
       </c>
@@ -2024,7 +2081,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="28" spans="1:10" hidden="1">
+    <row r="28" spans="1:12" hidden="1">
       <c r="A28" s="21" t="s">
         <v>93</v>
       </c>
@@ -2052,7 +2109,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="29" spans="1:10" hidden="1">
+    <row r="29" spans="1:12" hidden="1">
       <c r="A29" s="21" t="s">
         <v>94</v>
       </c>
@@ -2082,7 +2139,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="30" spans="1:10" hidden="1">
+    <row r="30" spans="1:12" hidden="1">
       <c r="A30" s="12" t="s">
         <v>95</v>
       </c>
@@ -2110,7 +2167,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="31" spans="1:10" hidden="1">
+    <row r="31" spans="1:12" hidden="1">
       <c r="A31" s="12" t="s">
         <v>96</v>
       </c>
@@ -2138,7 +2195,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="32" spans="1:10" hidden="1">
+    <row r="32" spans="1:12" hidden="1">
       <c r="A32" s="24" t="s">
         <v>97</v>
       </c>

</xml_diff>

<commit_message>
codigo e graficos sobre a instituicao de ensino.
</commit_message>
<xml_diff>
--- a/documentos/dataset_detalhes.xlsx
+++ b/documentos/dataset_detalhes.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="479" uniqueCount="176">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="488" uniqueCount="181">
   <si>
     <t>Sequencia</t>
   </si>
@@ -551,6 +551,21 @@
   </si>
   <si>
     <t>Maioria mora com familia</t>
+  </si>
+  <si>
+    <t>Maioria mudou (98%)</t>
+  </si>
+  <si>
+    <t>Maioria Não sei (62%</t>
+  </si>
+  <si>
+    <t>Não fazer grafico, data</t>
+  </si>
+  <si>
+    <t>Acesso a infra da Inst de Ensino pioraram (42%) ou ficou o mesmo (35%)</t>
+  </si>
+  <si>
+    <t>Maioria Sim, retornou todas as atividades</t>
   </si>
 </sst>
 </file>
@@ -586,7 +601,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="10">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -641,6 +656,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -655,7 +676,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="14" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
@@ -672,7 +693,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="14" fontId="2" fillId="3" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" quotePrefix="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -699,12 +719,16 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="8" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="14" fontId="2" fillId="8" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="9" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" quotePrefix="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="2" fillId="10" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1176,8 +1200,8 @@
   <dimension ref="A1:AZ69"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A20" sqref="A20"/>
+      <pane ySplit="1" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="K49" sqref="K49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1187,7 +1211,7 @@
     <col min="3" max="3" width="15.42578125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="10.42578125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="27.42578125" customWidth="1"/>
-    <col min="8" max="8" width="16.85546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="21" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="15" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="30.7109375" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="20.7109375" bestFit="1" customWidth="1"/>
@@ -1253,7 +1277,7 @@
       <c r="K2" s="6"/>
       <c r="L2" s="6"/>
     </row>
-    <row r="3" spans="1:52">
+    <row r="3" spans="1:52" hidden="1">
       <c r="A3" s="7" t="s">
         <v>68</v>
       </c>
@@ -1274,7 +1298,7 @@
       </c>
       <c r="G3" s="9"/>
       <c r="H3" s="9" t="s">
-        <v>122</v>
+        <v>124</v>
       </c>
       <c r="I3" s="9"/>
       <c r="J3" s="9" t="s">
@@ -1287,7 +1311,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="4" spans="1:52">
+    <row r="4" spans="1:52" hidden="1">
       <c r="A4" s="7" t="s">
         <v>69</v>
       </c>
@@ -1308,7 +1332,7 @@
       </c>
       <c r="G4" s="9"/>
       <c r="H4" s="9" t="s">
-        <v>122</v>
+        <v>124</v>
       </c>
       <c r="I4" s="9"/>
       <c r="J4" s="9" t="s">
@@ -1321,7 +1345,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="5" spans="1:52">
+    <row r="5" spans="1:52" hidden="1">
       <c r="A5" s="7" t="s">
         <v>70</v>
       </c>
@@ -1355,7 +1379,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="6" spans="1:52">
+    <row r="6" spans="1:52" hidden="1">
       <c r="A6" s="7" t="s">
         <v>71</v>
       </c>
@@ -1376,20 +1400,20 @@
       </c>
       <c r="G6" s="9"/>
       <c r="H6" s="9" t="s">
-        <v>122</v>
+        <v>124</v>
       </c>
       <c r="I6" s="9"/>
       <c r="J6" s="9" t="s">
         <v>142</v>
       </c>
-      <c r="K6" s="32" t="s">
+      <c r="K6" s="30" t="s">
         <v>9</v>
       </c>
-      <c r="L6" s="32" t="s">
+      <c r="L6" s="30" t="s">
         <v>165</v>
       </c>
     </row>
-    <row r="7" spans="1:52">
+    <row r="7" spans="1:52" hidden="1">
       <c r="A7" s="7" t="s">
         <v>72</v>
       </c>
@@ -1410,7 +1434,7 @@
       </c>
       <c r="G7" s="9"/>
       <c r="H7" s="9" t="s">
-        <v>122</v>
+        <v>124</v>
       </c>
       <c r="I7" s="9"/>
       <c r="J7" s="9" t="s">
@@ -1423,7 +1447,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="8" spans="1:52">
+    <row r="8" spans="1:52" hidden="1">
       <c r="A8" s="7" t="s">
         <v>73</v>
       </c>
@@ -1444,7 +1468,7 @@
       </c>
       <c r="G8" s="9"/>
       <c r="H8" s="9" t="s">
-        <v>122</v>
+        <v>124</v>
       </c>
       <c r="I8" s="9"/>
       <c r="J8" s="9" t="s">
@@ -1457,7 +1481,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="9" spans="1:52">
+    <row r="9" spans="1:52" hidden="1">
       <c r="A9" s="7" t="s">
         <v>74</v>
       </c>
@@ -1478,7 +1502,7 @@
       </c>
       <c r="G9" s="9"/>
       <c r="H9" s="9" t="s">
-        <v>122</v>
+        <v>124</v>
       </c>
       <c r="I9" s="9"/>
       <c r="J9" s="9" t="s">
@@ -1491,7 +1515,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="10" spans="1:52">
+    <row r="10" spans="1:52" hidden="1">
       <c r="A10" s="7" t="s">
         <v>75</v>
       </c>
@@ -1512,7 +1536,7 @@
       </c>
       <c r="G10" s="9"/>
       <c r="H10" s="9" t="s">
-        <v>122</v>
+        <v>124</v>
       </c>
       <c r="I10" s="9"/>
       <c r="J10" s="9" t="s">
@@ -1525,41 +1549,41 @@
         <v>167</v>
       </c>
     </row>
-    <row r="11" spans="1:52">
-      <c r="A11" s="7" t="s">
+    <row r="11" spans="1:52" hidden="1">
+      <c r="A11" s="31" t="s">
         <v>76</v>
       </c>
-      <c r="B11" s="10" t="s">
+      <c r="B11" s="32" t="s">
         <v>24</v>
       </c>
-      <c r="C11" s="9" t="s">
-        <v>123</v>
-      </c>
-      <c r="D11" s="9" t="s">
+      <c r="C11" s="33" t="s">
+        <v>123</v>
+      </c>
+      <c r="D11" s="33" t="s">
         <v>126</v>
       </c>
-      <c r="E11" s="9" t="s">
+      <c r="E11" s="33" t="s">
         <v>127</v>
       </c>
-      <c r="F11" s="9" t="s">
-        <v>8</v>
-      </c>
-      <c r="G11" s="9"/>
-      <c r="H11" s="9" t="s">
-        <v>122</v>
-      </c>
-      <c r="I11" s="9"/>
-      <c r="J11" s="9" t="s">
+      <c r="F11" s="33" t="s">
+        <v>8</v>
+      </c>
+      <c r="G11" s="33"/>
+      <c r="H11" s="33" t="s">
+        <v>178</v>
+      </c>
+      <c r="I11" s="33"/>
+      <c r="J11" s="33" t="s">
         <v>142</v>
       </c>
-      <c r="K11" s="9" t="s">
-        <v>12</v>
-      </c>
-      <c r="L11" s="9" t="s">
+      <c r="K11" s="33" t="s">
+        <v>12</v>
+      </c>
+      <c r="L11" s="33" t="s">
         <v>169</v>
       </c>
     </row>
-    <row r="12" spans="1:52">
+    <row r="12" spans="1:52" hidden="1">
       <c r="A12" s="7" t="s">
         <v>77</v>
       </c>
@@ -1580,7 +1604,7 @@
       </c>
       <c r="G12" s="9"/>
       <c r="H12" s="9" t="s">
-        <v>122</v>
+        <v>13</v>
       </c>
       <c r="I12" s="9"/>
       <c r="J12" s="9" t="s">
@@ -1593,7 +1617,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="13" spans="1:52">
+    <row r="13" spans="1:52" hidden="1">
       <c r="A13" s="7" t="s">
         <v>78</v>
       </c>
@@ -1627,92 +1651,106 @@
         <v>172</v>
       </c>
     </row>
-    <row r="14" spans="1:52" hidden="1">
-      <c r="A14" s="24" t="s">
+    <row r="14" spans="1:52">
+      <c r="A14" s="23" t="s">
         <v>79</v>
       </c>
-      <c r="B14" s="25" t="s">
+      <c r="B14" s="24" t="s">
         <v>27</v>
       </c>
-      <c r="C14" s="26" t="s">
-        <v>123</v>
-      </c>
-      <c r="D14" s="26" t="s">
-        <v>15</v>
-      </c>
-      <c r="E14" s="26" t="s">
-        <v>12</v>
-      </c>
-      <c r="F14" s="26" t="s">
-        <v>8</v>
-      </c>
-      <c r="G14" s="26"/>
-      <c r="H14" s="26" t="s">
+      <c r="C14" s="25" t="s">
+        <v>123</v>
+      </c>
+      <c r="D14" s="25" t="s">
+        <v>15</v>
+      </c>
+      <c r="E14" s="25" t="s">
+        <v>12</v>
+      </c>
+      <c r="F14" s="25" t="s">
+        <v>8</v>
+      </c>
+      <c r="G14" s="25"/>
+      <c r="H14" s="25" t="s">
         <v>13</v>
       </c>
-      <c r="I14" s="26"/>
-      <c r="J14" s="26" t="s">
+      <c r="I14" s="25"/>
+      <c r="J14" s="25" t="s">
         <v>134</v>
       </c>
-    </row>
-    <row r="15" spans="1:52" hidden="1">
-      <c r="A15" s="24" t="s">
+      <c r="K14" s="25" t="s">
+        <v>170</v>
+      </c>
+      <c r="L14" s="25" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="15" spans="1:52">
+      <c r="A15" s="23" t="s">
         <v>80</v>
       </c>
-      <c r="B15" s="25" t="s">
+      <c r="B15" s="24" t="s">
         <v>28</v>
       </c>
-      <c r="C15" s="26" t="s">
-        <v>123</v>
-      </c>
-      <c r="D15" s="26" t="s">
-        <v>15</v>
-      </c>
-      <c r="E15" s="26" t="s">
-        <v>12</v>
-      </c>
-      <c r="F15" s="26" t="s">
-        <v>8</v>
-      </c>
-      <c r="G15" s="26"/>
-      <c r="H15" s="26" t="s">
+      <c r="C15" s="25" t="s">
+        <v>123</v>
+      </c>
+      <c r="D15" s="25" t="s">
+        <v>15</v>
+      </c>
+      <c r="E15" s="25" t="s">
+        <v>12</v>
+      </c>
+      <c r="F15" s="25" t="s">
+        <v>8</v>
+      </c>
+      <c r="G15" s="25"/>
+      <c r="H15" s="25" t="s">
         <v>13</v>
       </c>
-      <c r="I15" s="26"/>
-      <c r="J15" s="26" t="s">
+      <c r="I15" s="25"/>
+      <c r="J15" s="25" t="s">
         <v>134</v>
       </c>
-    </row>
-    <row r="16" spans="1:52" hidden="1">
-      <c r="A16" s="24" t="s">
+      <c r="K15" s="25" t="s">
+        <v>170</v>
+      </c>
+      <c r="L15" s="25" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="16" spans="1:52">
+      <c r="A16" s="23" t="s">
         <v>81</v>
       </c>
-      <c r="B16" s="25" t="s">
+      <c r="B16" s="24" t="s">
         <v>29</v>
       </c>
-      <c r="C16" s="25" t="s">
+      <c r="C16" s="24" t="s">
         <v>120</v>
       </c>
-      <c r="D16" s="26" t="s">
-        <v>15</v>
-      </c>
-      <c r="E16" s="25" t="s">
-        <v>8</v>
-      </c>
-      <c r="F16" s="25" t="s">
-        <v>8</v>
-      </c>
-      <c r="G16" s="25"/>
-      <c r="H16" s="25" t="s">
+      <c r="D16" s="25" t="s">
+        <v>15</v>
+      </c>
+      <c r="E16" s="24" t="s">
+        <v>8</v>
+      </c>
+      <c r="F16" s="24" t="s">
+        <v>8</v>
+      </c>
+      <c r="G16" s="24"/>
+      <c r="H16" s="24" t="s">
         <v>18</v>
       </c>
-      <c r="I16" s="25" t="s">
+      <c r="I16" s="24" t="s">
         <v>132</v>
       </c>
-      <c r="J16" s="26" t="s">
+      <c r="J16" s="25" t="s">
         <v>134</v>
       </c>
-      <c r="K16" s="1"/>
+      <c r="K16" s="1" t="s">
+        <v>120</v>
+      </c>
       <c r="L16" s="1"/>
       <c r="M16" s="1"/>
       <c r="N16" s="1"/>
@@ -1755,35 +1793,37 @@
       <c r="AY16" s="1"/>
       <c r="AZ16" s="1"/>
     </row>
-    <row r="17" spans="1:12" hidden="1">
-      <c r="A17" s="24" t="s">
+    <row r="17" spans="1:12">
+      <c r="A17" s="31" t="s">
         <v>82</v>
       </c>
-      <c r="B17" s="27" t="s">
+      <c r="B17" s="32" t="s">
         <v>30</v>
       </c>
-      <c r="C17" s="26" t="s">
-        <v>123</v>
-      </c>
-      <c r="D17" s="26" t="s">
-        <v>15</v>
-      </c>
-      <c r="E17" s="26" t="s">
-        <v>12</v>
-      </c>
-      <c r="F17" s="26" t="s">
-        <v>8</v>
-      </c>
-      <c r="G17" s="26"/>
-      <c r="H17" s="26" t="s">
-        <v>13</v>
-      </c>
-      <c r="I17" s="26"/>
-      <c r="J17" s="26" t="s">
+      <c r="C17" s="33" t="s">
+        <v>123</v>
+      </c>
+      <c r="D17" s="33" t="s">
+        <v>15</v>
+      </c>
+      <c r="E17" s="33" t="s">
+        <v>12</v>
+      </c>
+      <c r="F17" s="33" t="s">
+        <v>8</v>
+      </c>
+      <c r="G17" s="33"/>
+      <c r="H17" s="33" t="s">
+        <v>178</v>
+      </c>
+      <c r="I17" s="33"/>
+      <c r="J17" s="33" t="s">
         <v>134</v>
       </c>
-    </row>
-    <row r="18" spans="1:12">
+      <c r="K17" s="33"/>
+      <c r="L17" s="33"/>
+    </row>
+    <row r="18" spans="1:12" hidden="1">
       <c r="A18" s="7" t="s">
         <v>83</v>
       </c>
@@ -1817,7 +1857,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="19" spans="1:12">
+    <row r="19" spans="1:12" hidden="1">
       <c r="A19" s="7" t="s">
         <v>84</v>
       </c>
@@ -1851,7 +1891,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="20" spans="1:12">
+    <row r="20" spans="1:12" hidden="1">
       <c r="A20" s="7" t="s">
         <v>85</v>
       </c>
@@ -1886,914 +1926,953 @@
       </c>
     </row>
     <row r="21" spans="1:12" hidden="1">
-      <c r="A21" s="21" t="s">
+      <c r="A21" s="20" t="s">
         <v>86</v>
       </c>
-      <c r="B21" s="22" t="s">
+      <c r="B21" s="21" t="s">
         <v>34</v>
       </c>
-      <c r="C21" s="23" t="s">
-        <v>123</v>
-      </c>
-      <c r="D21" s="23" t="s">
-        <v>15</v>
-      </c>
-      <c r="E21" s="23" t="s">
-        <v>12</v>
-      </c>
-      <c r="F21" s="23" t="s">
-        <v>8</v>
-      </c>
-      <c r="G21" s="23"/>
-      <c r="H21" s="23" t="s">
+      <c r="C21" s="22" t="s">
+        <v>123</v>
+      </c>
+      <c r="D21" s="22" t="s">
+        <v>15</v>
+      </c>
+      <c r="E21" s="22" t="s">
+        <v>12</v>
+      </c>
+      <c r="F21" s="22" t="s">
+        <v>8</v>
+      </c>
+      <c r="G21" s="22"/>
+      <c r="H21" s="22" t="s">
         <v>13</v>
       </c>
-      <c r="I21" s="23"/>
-      <c r="J21" s="23" t="s">
+      <c r="I21" s="22"/>
+      <c r="J21" s="22" t="s">
         <v>135</v>
       </c>
+      <c r="L21" s="25"/>
     </row>
     <row r="22" spans="1:12" hidden="1">
-      <c r="A22" s="21" t="s">
+      <c r="A22" s="20" t="s">
         <v>87</v>
       </c>
-      <c r="B22" s="22" t="s">
+      <c r="B22" s="21" t="s">
         <v>35</v>
       </c>
-      <c r="C22" s="23" t="s">
-        <v>123</v>
-      </c>
-      <c r="D22" s="23" t="s">
-        <v>15</v>
-      </c>
-      <c r="E22" s="23" t="s">
-        <v>12</v>
-      </c>
-      <c r="F22" s="23" t="s">
-        <v>8</v>
-      </c>
-      <c r="G22" s="23"/>
-      <c r="H22" s="23" t="s">
+      <c r="C22" s="22" t="s">
+        <v>123</v>
+      </c>
+      <c r="D22" s="22" t="s">
+        <v>15</v>
+      </c>
+      <c r="E22" s="22" t="s">
+        <v>12</v>
+      </c>
+      <c r="F22" s="22" t="s">
+        <v>8</v>
+      </c>
+      <c r="G22" s="22"/>
+      <c r="H22" s="22" t="s">
         <v>13</v>
       </c>
-      <c r="I22" s="23"/>
-      <c r="J22" s="23" t="s">
+      <c r="I22" s="22"/>
+      <c r="J22" s="22" t="s">
         <v>135</v>
       </c>
+      <c r="L22" s="25"/>
     </row>
     <row r="23" spans="1:12" hidden="1">
-      <c r="A23" s="21" t="s">
+      <c r="A23" s="20" t="s">
         <v>88</v>
       </c>
-      <c r="B23" s="22" t="s">
+      <c r="B23" s="21" t="s">
         <v>36</v>
       </c>
-      <c r="C23" s="23" t="s">
-        <v>123</v>
-      </c>
-      <c r="D23" s="23" t="s">
-        <v>15</v>
-      </c>
-      <c r="E23" s="23" t="s">
-        <v>12</v>
-      </c>
-      <c r="F23" s="23" t="s">
-        <v>8</v>
-      </c>
-      <c r="G23" s="23"/>
-      <c r="H23" s="23" t="s">
+      <c r="C23" s="22" t="s">
+        <v>123</v>
+      </c>
+      <c r="D23" s="22" t="s">
+        <v>15</v>
+      </c>
+      <c r="E23" s="22" t="s">
+        <v>12</v>
+      </c>
+      <c r="F23" s="22" t="s">
+        <v>8</v>
+      </c>
+      <c r="G23" s="22"/>
+      <c r="H23" s="22" t="s">
         <v>13</v>
       </c>
-      <c r="I23" s="23"/>
-      <c r="J23" s="23" t="s">
+      <c r="I23" s="22"/>
+      <c r="J23" s="22" t="s">
         <v>135</v>
       </c>
+      <c r="L23" s="25"/>
     </row>
     <row r="24" spans="1:12" hidden="1">
-      <c r="A24" s="21" t="s">
+      <c r="A24" s="20" t="s">
         <v>89</v>
       </c>
-      <c r="B24" s="22" t="s">
+      <c r="B24" s="21" t="s">
         <v>37</v>
       </c>
-      <c r="C24" s="23" t="s">
-        <v>123</v>
-      </c>
-      <c r="D24" s="23" t="s">
-        <v>15</v>
-      </c>
-      <c r="E24" s="23" t="s">
-        <v>12</v>
-      </c>
-      <c r="F24" s="23" t="s">
-        <v>8</v>
-      </c>
-      <c r="G24" s="23"/>
-      <c r="H24" s="23" t="s">
+      <c r="C24" s="22" t="s">
+        <v>123</v>
+      </c>
+      <c r="D24" s="22" t="s">
+        <v>15</v>
+      </c>
+      <c r="E24" s="22" t="s">
+        <v>12</v>
+      </c>
+      <c r="F24" s="22" t="s">
+        <v>8</v>
+      </c>
+      <c r="G24" s="22"/>
+      <c r="H24" s="22" t="s">
         <v>13</v>
       </c>
-      <c r="I24" s="23"/>
-      <c r="J24" s="23" t="s">
+      <c r="I24" s="22"/>
+      <c r="J24" s="22" t="s">
         <v>135</v>
       </c>
+      <c r="L24" s="25"/>
     </row>
     <row r="25" spans="1:12" hidden="1">
-      <c r="A25" s="21" t="s">
+      <c r="A25" s="20" t="s">
         <v>90</v>
       </c>
-      <c r="B25" s="22" t="s">
+      <c r="B25" s="21" t="s">
         <v>38</v>
       </c>
-      <c r="C25" s="23" t="s">
-        <v>123</v>
-      </c>
-      <c r="D25" s="23" t="s">
-        <v>15</v>
-      </c>
-      <c r="E25" s="23" t="s">
-        <v>12</v>
-      </c>
-      <c r="F25" s="23" t="s">
-        <v>8</v>
-      </c>
-      <c r="G25" s="23"/>
-      <c r="H25" s="23" t="s">
+      <c r="C25" s="22" t="s">
+        <v>123</v>
+      </c>
+      <c r="D25" s="22" t="s">
+        <v>15</v>
+      </c>
+      <c r="E25" s="22" t="s">
+        <v>12</v>
+      </c>
+      <c r="F25" s="22" t="s">
+        <v>8</v>
+      </c>
+      <c r="G25" s="22"/>
+      <c r="H25" s="22" t="s">
         <v>13</v>
       </c>
-      <c r="I25" s="23"/>
-      <c r="J25" s="23" t="s">
+      <c r="I25" s="22"/>
+      <c r="J25" s="22" t="s">
         <v>135</v>
       </c>
+      <c r="L25" s="25"/>
     </row>
     <row r="26" spans="1:12" hidden="1">
-      <c r="A26" s="12" t="s">
+      <c r="A26" s="11" t="s">
         <v>91</v>
       </c>
-      <c r="B26" s="13" t="s">
+      <c r="B26" s="12" t="s">
         <v>39</v>
       </c>
-      <c r="C26" s="14" t="s">
-        <v>123</v>
-      </c>
-      <c r="D26" s="14" t="s">
-        <v>15</v>
-      </c>
-      <c r="E26" s="14" t="s">
-        <v>12</v>
-      </c>
-      <c r="F26" s="14" t="s">
-        <v>8</v>
-      </c>
-      <c r="G26" s="14"/>
-      <c r="H26" s="14" t="s">
+      <c r="C26" s="13" t="s">
+        <v>123</v>
+      </c>
+      <c r="D26" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="E26" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="F26" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="G26" s="13"/>
+      <c r="H26" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="I26" s="14"/>
-      <c r="J26" s="14" t="s">
+      <c r="I26" s="13"/>
+      <c r="J26" s="13" t="s">
         <v>136</v>
       </c>
+      <c r="L26" s="25"/>
     </row>
     <row r="27" spans="1:12" hidden="1">
-      <c r="A27" s="15" t="s">
+      <c r="A27" s="14" t="s">
         <v>92</v>
       </c>
-      <c r="B27" s="16" t="s">
+      <c r="B27" s="15" t="s">
         <v>40</v>
       </c>
-      <c r="C27" s="17" t="s">
-        <v>123</v>
-      </c>
-      <c r="D27" s="17" t="s">
-        <v>15</v>
-      </c>
-      <c r="E27" s="17" t="s">
-        <v>12</v>
-      </c>
-      <c r="F27" s="17" t="s">
-        <v>8</v>
-      </c>
-      <c r="G27" s="17"/>
-      <c r="H27" s="17" t="s">
+      <c r="C27" s="16" t="s">
+        <v>123</v>
+      </c>
+      <c r="D27" s="16" t="s">
+        <v>15</v>
+      </c>
+      <c r="E27" s="16" t="s">
+        <v>12</v>
+      </c>
+      <c r="F27" s="16" t="s">
+        <v>8</v>
+      </c>
+      <c r="G27" s="16"/>
+      <c r="H27" s="16" t="s">
         <v>13</v>
       </c>
-      <c r="I27" s="17"/>
-      <c r="J27" s="17" t="s">
+      <c r="I27" s="16"/>
+      <c r="J27" s="16" t="s">
         <v>137</v>
       </c>
+      <c r="L27" s="25"/>
     </row>
     <row r="28" spans="1:12" hidden="1">
-      <c r="A28" s="21" t="s">
+      <c r="A28" s="20" t="s">
         <v>93</v>
       </c>
-      <c r="B28" s="22" t="s">
+      <c r="B28" s="21" t="s">
         <v>41</v>
       </c>
-      <c r="C28" s="23" t="s">
-        <v>123</v>
-      </c>
-      <c r="D28" s="23" t="s">
-        <v>15</v>
-      </c>
-      <c r="E28" s="23" t="s">
-        <v>12</v>
-      </c>
-      <c r="F28" s="23" t="s">
-        <v>8</v>
-      </c>
-      <c r="G28" s="23"/>
-      <c r="H28" s="23" t="s">
+      <c r="C28" s="22" t="s">
+        <v>123</v>
+      </c>
+      <c r="D28" s="22" t="s">
+        <v>15</v>
+      </c>
+      <c r="E28" s="22" t="s">
+        <v>12</v>
+      </c>
+      <c r="F28" s="22" t="s">
+        <v>8</v>
+      </c>
+      <c r="G28" s="22"/>
+      <c r="H28" s="22" t="s">
         <v>13</v>
       </c>
-      <c r="I28" s="23"/>
-      <c r="J28" s="23" t="s">
+      <c r="I28" s="22"/>
+      <c r="J28" s="22" t="s">
         <v>135</v>
       </c>
+      <c r="L28" s="25"/>
     </row>
     <row r="29" spans="1:12" hidden="1">
-      <c r="A29" s="21" t="s">
+      <c r="A29" s="20" t="s">
         <v>94</v>
       </c>
-      <c r="B29" s="22" t="s">
+      <c r="B29" s="21" t="s">
         <v>42</v>
       </c>
-      <c r="C29" s="22" t="s">
+      <c r="C29" s="21" t="s">
         <v>120</v>
       </c>
-      <c r="D29" s="23" t="s">
-        <v>15</v>
-      </c>
-      <c r="E29" s="22" t="s">
-        <v>8</v>
-      </c>
-      <c r="F29" s="22" t="s">
-        <v>8</v>
-      </c>
-      <c r="G29" s="22"/>
-      <c r="H29" s="22" t="s">
+      <c r="D29" s="22" t="s">
+        <v>15</v>
+      </c>
+      <c r="E29" s="21" t="s">
+        <v>8</v>
+      </c>
+      <c r="F29" s="21" t="s">
+        <v>8</v>
+      </c>
+      <c r="G29" s="21"/>
+      <c r="H29" s="21" t="s">
         <v>18</v>
       </c>
-      <c r="I29" s="22" t="s">
+      <c r="I29" s="21" t="s">
         <v>132</v>
       </c>
-      <c r="J29" s="23" t="s">
+      <c r="J29" s="22" t="s">
         <v>135</v>
       </c>
+      <c r="L29" s="25"/>
     </row>
     <row r="30" spans="1:12" hidden="1">
-      <c r="A30" s="12" t="s">
+      <c r="A30" s="11" t="s">
         <v>95</v>
       </c>
-      <c r="B30" s="13" t="s">
+      <c r="B30" s="12" t="s">
         <v>43</v>
       </c>
-      <c r="C30" s="14" t="s">
-        <v>123</v>
-      </c>
-      <c r="D30" s="14" t="s">
-        <v>15</v>
-      </c>
-      <c r="E30" s="14" t="s">
-        <v>12</v>
-      </c>
-      <c r="F30" s="14" t="s">
-        <v>8</v>
-      </c>
-      <c r="G30" s="14"/>
-      <c r="H30" s="14" t="s">
+      <c r="C30" s="13" t="s">
+        <v>123</v>
+      </c>
+      <c r="D30" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="E30" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="F30" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="G30" s="13"/>
+      <c r="H30" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="I30" s="14"/>
-      <c r="J30" s="14" t="s">
+      <c r="I30" s="13"/>
+      <c r="J30" s="13" t="s">
         <v>136</v>
       </c>
+      <c r="L30" s="25"/>
     </row>
     <row r="31" spans="1:12" hidden="1">
-      <c r="A31" s="12" t="s">
+      <c r="A31" s="11" t="s">
         <v>96</v>
       </c>
-      <c r="B31" s="13" t="s">
+      <c r="B31" s="12" t="s">
         <v>44</v>
       </c>
-      <c r="C31" s="14" t="s">
-        <v>123</v>
-      </c>
-      <c r="D31" s="14" t="s">
-        <v>15</v>
-      </c>
-      <c r="E31" s="14" t="s">
-        <v>12</v>
-      </c>
-      <c r="F31" s="14" t="s">
-        <v>8</v>
-      </c>
-      <c r="G31" s="14"/>
-      <c r="H31" s="14" t="s">
+      <c r="C31" s="13" t="s">
+        <v>123</v>
+      </c>
+      <c r="D31" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="E31" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="F31" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="G31" s="13"/>
+      <c r="H31" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="I31" s="14"/>
-      <c r="J31" s="14" t="s">
+      <c r="I31" s="13"/>
+      <c r="J31" s="13" t="s">
         <v>136</v>
       </c>
-    </row>
-    <row r="32" spans="1:12" hidden="1">
-      <c r="A32" s="24" t="s">
+      <c r="L31" s="25"/>
+    </row>
+    <row r="32" spans="1:12">
+      <c r="A32" s="23" t="s">
         <v>97</v>
       </c>
-      <c r="B32" s="25" t="s">
+      <c r="B32" s="24" t="s">
         <v>45</v>
       </c>
-      <c r="C32" s="26" t="s">
-        <v>123</v>
-      </c>
-      <c r="D32" s="26" t="s">
-        <v>15</v>
-      </c>
-      <c r="E32" s="26" t="s">
-        <v>12</v>
-      </c>
-      <c r="F32" s="26" t="s">
-        <v>8</v>
-      </c>
-      <c r="G32" s="26"/>
-      <c r="H32" s="26" t="s">
+      <c r="C32" s="25" t="s">
+        <v>123</v>
+      </c>
+      <c r="D32" s="25" t="s">
+        <v>15</v>
+      </c>
+      <c r="E32" s="25" t="s">
+        <v>12</v>
+      </c>
+      <c r="F32" s="25" t="s">
+        <v>8</v>
+      </c>
+      <c r="G32" s="25"/>
+      <c r="H32" s="25" t="s">
         <v>13</v>
       </c>
-      <c r="I32" s="26"/>
-      <c r="J32" s="26" t="s">
+      <c r="I32" s="25"/>
+      <c r="J32" s="25" t="s">
         <v>134</v>
       </c>
-    </row>
-    <row r="33" spans="1:10" hidden="1">
-      <c r="A33" s="12" t="s">
+      <c r="K32" s="25" t="s">
+        <v>9</v>
+      </c>
+      <c r="L32" s="25" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="33" spans="1:12" hidden="1">
+      <c r="A33" s="11" t="s">
         <v>98</v>
       </c>
-      <c r="B33" s="13" t="s">
+      <c r="B33" s="12" t="s">
         <v>46</v>
       </c>
-      <c r="C33" s="14" t="s">
-        <v>123</v>
-      </c>
-      <c r="D33" s="14" t="s">
-        <v>15</v>
-      </c>
-      <c r="E33" s="14" t="s">
-        <v>12</v>
-      </c>
-      <c r="F33" s="14" t="s">
-        <v>8</v>
-      </c>
-      <c r="G33" s="14"/>
-      <c r="H33" s="14" t="s">
+      <c r="C33" s="13" t="s">
+        <v>123</v>
+      </c>
+      <c r="D33" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="E33" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="F33" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="G33" s="13"/>
+      <c r="H33" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="I33" s="14"/>
-      <c r="J33" s="14" t="s">
+      <c r="I33" s="13"/>
+      <c r="J33" s="13" t="s">
         <v>136</v>
       </c>
-    </row>
-    <row r="34" spans="1:10" hidden="1">
-      <c r="A34" s="12" t="s">
+      <c r="L33" s="25"/>
+    </row>
+    <row r="34" spans="1:12" hidden="1">
+      <c r="A34" s="11" t="s">
         <v>99</v>
       </c>
-      <c r="B34" s="13" t="s">
+      <c r="B34" s="12" t="s">
         <v>47</v>
       </c>
-      <c r="C34" s="14" t="s">
-        <v>123</v>
-      </c>
-      <c r="D34" s="14" t="s">
-        <v>15</v>
-      </c>
-      <c r="E34" s="14" t="s">
-        <v>12</v>
-      </c>
-      <c r="F34" s="14" t="s">
-        <v>8</v>
-      </c>
-      <c r="G34" s="14"/>
-      <c r="H34" s="14" t="s">
+      <c r="C34" s="13" t="s">
+        <v>123</v>
+      </c>
+      <c r="D34" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="E34" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="F34" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="G34" s="13"/>
+      <c r="H34" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="I34" s="14"/>
-      <c r="J34" s="14" t="s">
+      <c r="I34" s="13"/>
+      <c r="J34" s="13" t="s">
         <v>136</v>
       </c>
-    </row>
-    <row r="35" spans="1:10" hidden="1">
-      <c r="A35" s="12" t="s">
+      <c r="L34" s="25"/>
+    </row>
+    <row r="35" spans="1:12" hidden="1">
+      <c r="A35" s="11" t="s">
         <v>100</v>
       </c>
-      <c r="B35" s="13" t="s">
+      <c r="B35" s="12" t="s">
         <v>48</v>
       </c>
-      <c r="C35" s="14" t="s">
-        <v>123</v>
-      </c>
-      <c r="D35" s="14" t="s">
-        <v>15</v>
-      </c>
-      <c r="E35" s="14" t="s">
-        <v>12</v>
-      </c>
-      <c r="F35" s="14" t="s">
-        <v>8</v>
-      </c>
-      <c r="G35" s="14"/>
-      <c r="H35" s="14" t="s">
+      <c r="C35" s="13" t="s">
+        <v>123</v>
+      </c>
+      <c r="D35" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="E35" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="F35" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="G35" s="13"/>
+      <c r="H35" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="I35" s="14"/>
-      <c r="J35" s="14" t="s">
+      <c r="I35" s="13"/>
+      <c r="J35" s="13" t="s">
         <v>136</v>
       </c>
-    </row>
-    <row r="36" spans="1:10" hidden="1">
-      <c r="A36" s="24" t="s">
+      <c r="L35" s="25"/>
+    </row>
+    <row r="36" spans="1:12">
+      <c r="A36" s="23" t="s">
         <v>101</v>
       </c>
-      <c r="B36" s="25" t="s">
+      <c r="B36" s="24" t="s">
         <v>49</v>
       </c>
-      <c r="C36" s="26" t="s">
-        <v>123</v>
-      </c>
-      <c r="D36" s="26" t="s">
-        <v>15</v>
-      </c>
-      <c r="E36" s="26" t="s">
-        <v>12</v>
-      </c>
-      <c r="F36" s="26" t="s">
-        <v>8</v>
-      </c>
-      <c r="G36" s="26"/>
-      <c r="H36" s="26" t="s">
+      <c r="C36" s="25" t="s">
+        <v>123</v>
+      </c>
+      <c r="D36" s="25" t="s">
+        <v>15</v>
+      </c>
+      <c r="E36" s="25" t="s">
+        <v>12</v>
+      </c>
+      <c r="F36" s="25" t="s">
+        <v>8</v>
+      </c>
+      <c r="G36" s="25"/>
+      <c r="H36" s="25" t="s">
         <v>13</v>
       </c>
-      <c r="I36" s="26"/>
-      <c r="J36" s="26" t="s">
+      <c r="I36" s="25"/>
+      <c r="J36" s="25" t="s">
         <v>134</v>
       </c>
-    </row>
-    <row r="37" spans="1:10" hidden="1">
-      <c r="A37" s="24" t="s">
+      <c r="K36" s="25" t="s">
+        <v>9</v>
+      </c>
+      <c r="L36" s="25" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="37" spans="1:12">
+      <c r="A37" s="23" t="s">
         <v>102</v>
       </c>
-      <c r="B37" s="25" t="s">
+      <c r="B37" s="24" t="s">
         <v>50</v>
       </c>
-      <c r="C37" s="26" t="s">
-        <v>123</v>
-      </c>
-      <c r="D37" s="26" t="s">
-        <v>15</v>
-      </c>
-      <c r="E37" s="26" t="s">
-        <v>12</v>
-      </c>
-      <c r="F37" s="26" t="s">
-        <v>8</v>
-      </c>
-      <c r="G37" s="26"/>
-      <c r="H37" s="26" t="s">
+      <c r="C37" s="25" t="s">
+        <v>123</v>
+      </c>
+      <c r="D37" s="25" t="s">
+        <v>15</v>
+      </c>
+      <c r="E37" s="25" t="s">
+        <v>12</v>
+      </c>
+      <c r="F37" s="25" t="s">
+        <v>8</v>
+      </c>
+      <c r="G37" s="25"/>
+      <c r="H37" s="25" t="s">
         <v>13</v>
       </c>
-      <c r="I37" s="26"/>
-      <c r="J37" s="26" t="s">
+      <c r="I37" s="25"/>
+      <c r="J37" s="25" t="s">
         <v>134</v>
       </c>
-    </row>
-    <row r="38" spans="1:10" hidden="1">
-      <c r="A38" s="21" t="s">
+      <c r="L37" s="25"/>
+    </row>
+    <row r="38" spans="1:12" hidden="1">
+      <c r="A38" s="20" t="s">
         <v>103</v>
       </c>
-      <c r="B38" s="22" t="s">
+      <c r="B38" s="21" t="s">
         <v>51</v>
       </c>
-      <c r="C38" s="23" t="s">
-        <v>123</v>
-      </c>
-      <c r="D38" s="23" t="s">
-        <v>15</v>
-      </c>
-      <c r="E38" s="23" t="s">
-        <v>12</v>
-      </c>
-      <c r="F38" s="23" t="s">
-        <v>8</v>
-      </c>
-      <c r="G38" s="23"/>
-      <c r="H38" s="23" t="s">
+      <c r="C38" s="22" t="s">
+        <v>123</v>
+      </c>
+      <c r="D38" s="22" t="s">
+        <v>15</v>
+      </c>
+      <c r="E38" s="22" t="s">
+        <v>12</v>
+      </c>
+      <c r="F38" s="22" t="s">
+        <v>8</v>
+      </c>
+      <c r="G38" s="22"/>
+      <c r="H38" s="22" t="s">
         <v>13</v>
       </c>
-      <c r="I38" s="23"/>
-      <c r="J38" s="23" t="s">
+      <c r="I38" s="22"/>
+      <c r="J38" s="22" t="s">
         <v>138</v>
       </c>
-    </row>
-    <row r="39" spans="1:10" hidden="1">
-      <c r="A39" s="12" t="s">
+      <c r="L38" s="25"/>
+    </row>
+    <row r="39" spans="1:12" hidden="1">
+      <c r="A39" s="11" t="s">
         <v>104</v>
       </c>
-      <c r="B39" s="13" t="s">
+      <c r="B39" s="12" t="s">
         <v>52</v>
       </c>
-      <c r="C39" s="13" t="s">
+      <c r="C39" s="12" t="s">
         <v>120</v>
       </c>
-      <c r="D39" s="14" t="s">
-        <v>15</v>
-      </c>
-      <c r="E39" s="13" t="s">
-        <v>8</v>
-      </c>
-      <c r="F39" s="13" t="s">
-        <v>8</v>
-      </c>
-      <c r="G39" s="13"/>
-      <c r="H39" s="13" t="s">
+      <c r="D39" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="E39" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="F39" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="G39" s="12"/>
+      <c r="H39" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="I39" s="13" t="s">
+      <c r="I39" s="12" t="s">
         <v>132</v>
       </c>
-      <c r="J39" s="14" t="s">
+      <c r="J39" s="13" t="s">
         <v>136</v>
       </c>
-    </row>
-    <row r="40" spans="1:10" hidden="1">
-      <c r="A40" s="18" t="s">
+      <c r="L39" s="25"/>
+    </row>
+    <row r="40" spans="1:12" hidden="1">
+      <c r="A40" s="17" t="s">
         <v>105</v>
       </c>
-      <c r="B40" s="19" t="s">
+      <c r="B40" s="18" t="s">
         <v>53</v>
       </c>
-      <c r="C40" s="20" t="s">
-        <v>123</v>
-      </c>
-      <c r="D40" s="20" t="s">
-        <v>15</v>
-      </c>
-      <c r="E40" s="20" t="s">
-        <v>12</v>
-      </c>
-      <c r="F40" s="20" t="s">
-        <v>8</v>
-      </c>
-      <c r="G40" s="20"/>
-      <c r="H40" s="20" t="s">
+      <c r="C40" s="19" t="s">
+        <v>123</v>
+      </c>
+      <c r="D40" s="19" t="s">
+        <v>15</v>
+      </c>
+      <c r="E40" s="19" t="s">
+        <v>12</v>
+      </c>
+      <c r="F40" s="19" t="s">
+        <v>8</v>
+      </c>
+      <c r="G40" s="19"/>
+      <c r="H40" s="19" t="s">
         <v>13</v>
       </c>
-      <c r="I40" s="20"/>
-      <c r="J40" s="20" t="s">
+      <c r="I40" s="19"/>
+      <c r="J40" s="19" t="s">
         <v>139</v>
       </c>
-    </row>
-    <row r="41" spans="1:10" hidden="1">
-      <c r="A41" s="18" t="s">
+      <c r="L40" s="25"/>
+    </row>
+    <row r="41" spans="1:12" hidden="1">
+      <c r="A41" s="17" t="s">
         <v>106</v>
       </c>
-      <c r="B41" s="19" t="s">
+      <c r="B41" s="18" t="s">
         <v>54</v>
       </c>
-      <c r="C41" s="20" t="s">
-        <v>123</v>
-      </c>
-      <c r="D41" s="20" t="s">
-        <v>15</v>
-      </c>
-      <c r="E41" s="20" t="s">
-        <v>12</v>
-      </c>
-      <c r="F41" s="20" t="s">
-        <v>8</v>
-      </c>
-      <c r="G41" s="20"/>
-      <c r="H41" s="20" t="s">
+      <c r="C41" s="19" t="s">
+        <v>123</v>
+      </c>
+      <c r="D41" s="19" t="s">
+        <v>15</v>
+      </c>
+      <c r="E41" s="19" t="s">
+        <v>12</v>
+      </c>
+      <c r="F41" s="19" t="s">
+        <v>8</v>
+      </c>
+      <c r="G41" s="19"/>
+      <c r="H41" s="19" t="s">
         <v>13</v>
       </c>
-      <c r="I41" s="20"/>
-      <c r="J41" s="20" t="s">
+      <c r="I41" s="19"/>
+      <c r="J41" s="19" t="s">
         <v>139</v>
       </c>
-    </row>
-    <row r="42" spans="1:10" hidden="1">
-      <c r="A42" s="18" t="s">
+      <c r="L41" s="25"/>
+    </row>
+    <row r="42" spans="1:12" hidden="1">
+      <c r="A42" s="17" t="s">
         <v>107</v>
       </c>
-      <c r="B42" s="19" t="s">
+      <c r="B42" s="18" t="s">
         <v>55</v>
       </c>
-      <c r="C42" s="20" t="s">
-        <v>123</v>
-      </c>
-      <c r="D42" s="20" t="s">
-        <v>15</v>
-      </c>
-      <c r="E42" s="20" t="s">
-        <v>12</v>
-      </c>
-      <c r="F42" s="20" t="s">
-        <v>8</v>
-      </c>
-      <c r="G42" s="20"/>
-      <c r="H42" s="20" t="s">
+      <c r="C42" s="19" t="s">
+        <v>123</v>
+      </c>
+      <c r="D42" s="19" t="s">
+        <v>15</v>
+      </c>
+      <c r="E42" s="19" t="s">
+        <v>12</v>
+      </c>
+      <c r="F42" s="19" t="s">
+        <v>8</v>
+      </c>
+      <c r="G42" s="19"/>
+      <c r="H42" s="19" t="s">
         <v>13</v>
       </c>
-      <c r="I42" s="20"/>
-      <c r="J42" s="20" t="s">
+      <c r="I42" s="19"/>
+      <c r="J42" s="19" t="s">
         <v>139</v>
       </c>
-    </row>
-    <row r="43" spans="1:10" hidden="1">
-      <c r="A43" s="18" t="s">
+      <c r="L42" s="25"/>
+    </row>
+    <row r="43" spans="1:12" hidden="1">
+      <c r="A43" s="17" t="s">
         <v>108</v>
       </c>
-      <c r="B43" s="19" t="s">
+      <c r="B43" s="18" t="s">
         <v>56</v>
       </c>
-      <c r="C43" s="20" t="s">
-        <v>123</v>
-      </c>
-      <c r="D43" s="20" t="s">
-        <v>15</v>
-      </c>
-      <c r="E43" s="20" t="s">
-        <v>12</v>
-      </c>
-      <c r="F43" s="20" t="s">
-        <v>8</v>
-      </c>
-      <c r="G43" s="20"/>
-      <c r="H43" s="20" t="s">
+      <c r="C43" s="19" t="s">
+        <v>123</v>
+      </c>
+      <c r="D43" s="19" t="s">
+        <v>15</v>
+      </c>
+      <c r="E43" s="19" t="s">
+        <v>12</v>
+      </c>
+      <c r="F43" s="19" t="s">
+        <v>8</v>
+      </c>
+      <c r="G43" s="19"/>
+      <c r="H43" s="19" t="s">
         <v>13</v>
       </c>
-      <c r="I43" s="20"/>
-      <c r="J43" s="20" t="s">
+      <c r="I43" s="19"/>
+      <c r="J43" s="19" t="s">
         <v>139</v>
       </c>
-    </row>
-    <row r="44" spans="1:10" hidden="1">
-      <c r="A44" s="18" t="s">
+      <c r="L43" s="25"/>
+    </row>
+    <row r="44" spans="1:12" hidden="1">
+      <c r="A44" s="17" t="s">
         <v>109</v>
       </c>
-      <c r="B44" s="19" t="s">
+      <c r="B44" s="18" t="s">
         <v>57</v>
       </c>
-      <c r="C44" s="20" t="s">
-        <v>123</v>
-      </c>
-      <c r="D44" s="20" t="s">
-        <v>15</v>
-      </c>
-      <c r="E44" s="20" t="s">
+      <c r="C44" s="19" t="s">
+        <v>123</v>
+      </c>
+      <c r="D44" s="19" t="s">
+        <v>15</v>
+      </c>
+      <c r="E44" s="19" t="s">
         <v>133</v>
       </c>
-      <c r="F44" s="20" t="s">
-        <v>8</v>
-      </c>
-      <c r="G44" s="20"/>
-      <c r="H44" s="20" t="s">
+      <c r="F44" s="19" t="s">
+        <v>8</v>
+      </c>
+      <c r="G44" s="19"/>
+      <c r="H44" s="19" t="s">
         <v>122</v>
       </c>
-      <c r="I44" s="20"/>
-      <c r="J44" s="20" t="s">
+      <c r="I44" s="19"/>
+      <c r="J44" s="19" t="s">
         <v>139</v>
       </c>
-    </row>
-    <row r="45" spans="1:10" hidden="1">
-      <c r="A45" s="18" t="s">
+      <c r="L44" s="25"/>
+    </row>
+    <row r="45" spans="1:12" hidden="1">
+      <c r="A45" s="17" t="s">
         <v>110</v>
       </c>
-      <c r="B45" s="19" t="s">
+      <c r="B45" s="18" t="s">
         <v>58</v>
       </c>
-      <c r="C45" s="19" t="s">
+      <c r="C45" s="18" t="s">
         <v>120</v>
       </c>
-      <c r="D45" s="20" t="s">
-        <v>15</v>
-      </c>
-      <c r="E45" s="19" t="s">
-        <v>8</v>
-      </c>
-      <c r="F45" s="19" t="s">
-        <v>8</v>
-      </c>
-      <c r="G45" s="19"/>
-      <c r="H45" s="19" t="s">
+      <c r="D45" s="19" t="s">
+        <v>15</v>
+      </c>
+      <c r="E45" s="18" t="s">
+        <v>8</v>
+      </c>
+      <c r="F45" s="18" t="s">
+        <v>8</v>
+      </c>
+      <c r="G45" s="18"/>
+      <c r="H45" s="18" t="s">
         <v>18</v>
       </c>
-      <c r="I45" s="19" t="s">
+      <c r="I45" s="18" t="s">
         <v>132</v>
       </c>
-      <c r="J45" s="20" t="s">
+      <c r="J45" s="19" t="s">
         <v>139</v>
       </c>
-    </row>
-    <row r="46" spans="1:10" hidden="1">
-      <c r="A46" s="24" t="s">
+      <c r="L45" s="25"/>
+    </row>
+    <row r="46" spans="1:12">
+      <c r="A46" s="23" t="s">
         <v>111</v>
       </c>
-      <c r="B46" s="25" t="s">
+      <c r="B46" s="24" t="s">
         <v>59</v>
       </c>
-      <c r="C46" s="26" t="s">
-        <v>123</v>
-      </c>
-      <c r="D46" s="26" t="s">
-        <v>15</v>
-      </c>
-      <c r="E46" s="26" t="s">
-        <v>12</v>
-      </c>
-      <c r="F46" s="26" t="s">
-        <v>8</v>
-      </c>
-      <c r="G46" s="26"/>
-      <c r="H46" s="26" t="s">
+      <c r="C46" s="25" t="s">
+        <v>123</v>
+      </c>
+      <c r="D46" s="25" t="s">
+        <v>15</v>
+      </c>
+      <c r="E46" s="25" t="s">
+        <v>12</v>
+      </c>
+      <c r="F46" s="25" t="s">
+        <v>8</v>
+      </c>
+      <c r="G46" s="25"/>
+      <c r="H46" s="25" t="s">
         <v>13</v>
       </c>
-      <c r="I46" s="26"/>
-      <c r="J46" s="26" t="s">
+      <c r="I46" s="25"/>
+      <c r="J46" s="25" t="s">
         <v>134</v>
       </c>
-    </row>
-    <row r="47" spans="1:10" hidden="1">
-      <c r="A47" s="24" t="s">
+      <c r="L46" s="25"/>
+    </row>
+    <row r="47" spans="1:12">
+      <c r="A47" s="23" t="s">
         <v>112</v>
       </c>
-      <c r="B47" s="25" t="s">
+      <c r="B47" s="24" t="s">
         <v>60</v>
       </c>
-      <c r="C47" s="25" t="s">
+      <c r="C47" s="24" t="s">
         <v>120</v>
       </c>
-      <c r="D47" s="26" t="s">
-        <v>15</v>
-      </c>
-      <c r="E47" s="25" t="s">
-        <v>8</v>
-      </c>
-      <c r="F47" s="25" t="s">
-        <v>8</v>
-      </c>
-      <c r="G47" s="25"/>
-      <c r="H47" s="25" t="s">
+      <c r="D47" s="25" t="s">
+        <v>15</v>
+      </c>
+      <c r="E47" s="24" t="s">
+        <v>8</v>
+      </c>
+      <c r="F47" s="24" t="s">
+        <v>8</v>
+      </c>
+      <c r="G47" s="24"/>
+      <c r="H47" s="24" t="s">
         <v>18</v>
       </c>
-      <c r="I47" s="25" t="s">
+      <c r="I47" s="24" t="s">
         <v>132</v>
       </c>
-      <c r="J47" s="26" t="s">
+      <c r="J47" s="25" t="s">
         <v>134</v>
       </c>
-    </row>
-    <row r="48" spans="1:10" hidden="1">
-      <c r="A48" s="24" t="s">
+      <c r="L47" s="25"/>
+    </row>
+    <row r="48" spans="1:12">
+      <c r="A48" s="23" t="s">
         <v>113</v>
       </c>
-      <c r="B48" s="25" t="s">
+      <c r="B48" s="24" t="s">
         <v>61</v>
       </c>
-      <c r="C48" s="25" t="s">
+      <c r="C48" s="24" t="s">
         <v>120</v>
       </c>
-      <c r="D48" s="26" t="s">
-        <v>15</v>
-      </c>
-      <c r="E48" s="25" t="s">
-        <v>8</v>
-      </c>
-      <c r="F48" s="25" t="s">
-        <v>8</v>
-      </c>
-      <c r="G48" s="25"/>
-      <c r="H48" s="25" t="s">
+      <c r="D48" s="25" t="s">
+        <v>15</v>
+      </c>
+      <c r="E48" s="24" t="s">
+        <v>8</v>
+      </c>
+      <c r="F48" s="24" t="s">
+        <v>8</v>
+      </c>
+      <c r="G48" s="24"/>
+      <c r="H48" s="24" t="s">
         <v>18</v>
       </c>
-      <c r="I48" s="25" t="s">
+      <c r="I48" s="24" t="s">
         <v>132</v>
       </c>
-      <c r="J48" s="26" t="s">
+      <c r="J48" s="25" t="s">
         <v>134</v>
       </c>
-    </row>
-    <row r="49" spans="1:10" hidden="1">
-      <c r="A49" s="24" t="s">
+      <c r="L48" s="25"/>
+    </row>
+    <row r="49" spans="1:12">
+      <c r="A49" s="23" t="s">
         <v>114</v>
       </c>
-      <c r="B49" s="25" t="s">
+      <c r="B49" s="24" t="s">
         <v>62</v>
       </c>
-      <c r="C49" s="25" t="s">
+      <c r="C49" s="24" t="s">
         <v>120</v>
       </c>
-      <c r="D49" s="26" t="s">
-        <v>15</v>
-      </c>
-      <c r="E49" s="25" t="s">
-        <v>8</v>
-      </c>
-      <c r="F49" s="25" t="s">
-        <v>8</v>
-      </c>
-      <c r="G49" s="25"/>
-      <c r="H49" s="25" t="s">
+      <c r="D49" s="25" t="s">
+        <v>15</v>
+      </c>
+      <c r="E49" s="24" t="s">
+        <v>8</v>
+      </c>
+      <c r="F49" s="24" t="s">
+        <v>8</v>
+      </c>
+      <c r="G49" s="24"/>
+      <c r="H49" s="24" t="s">
         <v>18</v>
       </c>
-      <c r="I49" s="25" t="s">
+      <c r="I49" s="24" t="s">
         <v>132</v>
       </c>
-      <c r="J49" s="26" t="s">
+      <c r="J49" s="25" t="s">
         <v>134</v>
       </c>
-    </row>
-    <row r="50" spans="1:10" hidden="1">
-      <c r="A50" s="21" t="s">
+      <c r="L49" s="25"/>
+    </row>
+    <row r="50" spans="1:12" hidden="1">
+      <c r="A50" s="20" t="s">
         <v>115</v>
       </c>
-      <c r="B50" s="22" t="s">
+      <c r="B50" s="21" t="s">
         <v>63</v>
       </c>
-      <c r="C50" s="23" t="s">
-        <v>123</v>
-      </c>
-      <c r="D50" s="23" t="s">
-        <v>15</v>
-      </c>
-      <c r="E50" s="23" t="s">
-        <v>12</v>
-      </c>
-      <c r="F50" s="23" t="s">
-        <v>8</v>
-      </c>
-      <c r="G50" s="23"/>
-      <c r="H50" s="23" t="s">
+      <c r="C50" s="22" t="s">
+        <v>123</v>
+      </c>
+      <c r="D50" s="22" t="s">
+        <v>15</v>
+      </c>
+      <c r="E50" s="22" t="s">
+        <v>12</v>
+      </c>
+      <c r="F50" s="22" t="s">
+        <v>8</v>
+      </c>
+      <c r="G50" s="22"/>
+      <c r="H50" s="22" t="s">
         <v>13</v>
       </c>
-      <c r="I50" s="23"/>
-      <c r="J50" s="23" t="s">
+      <c r="I50" s="22"/>
+      <c r="J50" s="22" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="51" spans="1:10" hidden="1">
-      <c r="A51" s="21" t="s">
+    <row r="51" spans="1:12" hidden="1">
+      <c r="A51" s="20" t="s">
         <v>116</v>
       </c>
-      <c r="B51" s="22" t="s">
+      <c r="B51" s="21" t="s">
         <v>64</v>
       </c>
-      <c r="C51" s="23" t="s">
-        <v>123</v>
-      </c>
-      <c r="D51" s="23" t="s">
-        <v>15</v>
-      </c>
-      <c r="E51" s="23" t="s">
-        <v>12</v>
-      </c>
-      <c r="F51" s="23" t="s">
-        <v>8</v>
-      </c>
-      <c r="G51" s="23"/>
-      <c r="H51" s="23" t="s">
+      <c r="C51" s="22" t="s">
+        <v>123</v>
+      </c>
+      <c r="D51" s="22" t="s">
+        <v>15</v>
+      </c>
+      <c r="E51" s="22" t="s">
+        <v>12</v>
+      </c>
+      <c r="F51" s="22" t="s">
+        <v>8</v>
+      </c>
+      <c r="G51" s="22"/>
+      <c r="H51" s="22" t="s">
         <v>13</v>
       </c>
-      <c r="I51" s="23"/>
-      <c r="J51" s="23" t="s">
+      <c r="I51" s="22"/>
+      <c r="J51" s="22" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="52" spans="1:10" hidden="1">
-      <c r="A52" s="21" t="s">
+    <row r="52" spans="1:12" hidden="1">
+      <c r="A52" s="20" t="s">
         <v>117</v>
       </c>
-      <c r="B52" s="22" t="s">
+      <c r="B52" s="21" t="s">
         <v>65</v>
       </c>
-      <c r="C52" s="23" t="s">
-        <v>123</v>
-      </c>
-      <c r="D52" s="23" t="s">
-        <v>15</v>
-      </c>
-      <c r="E52" s="23" t="s">
-        <v>12</v>
-      </c>
-      <c r="F52" s="23" t="s">
-        <v>8</v>
-      </c>
-      <c r="G52" s="23"/>
-      <c r="H52" s="23" t="s">
+      <c r="C52" s="22" t="s">
+        <v>123</v>
+      </c>
+      <c r="D52" s="22" t="s">
+        <v>15</v>
+      </c>
+      <c r="E52" s="22" t="s">
+        <v>12</v>
+      </c>
+      <c r="F52" s="22" t="s">
+        <v>8</v>
+      </c>
+      <c r="G52" s="22"/>
+      <c r="H52" s="22" t="s">
         <v>13</v>
       </c>
-      <c r="I52" s="23"/>
-      <c r="J52" s="23" t="s">
+      <c r="I52" s="22"/>
+      <c r="J52" s="22" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="53" spans="1:10" hidden="1">
+    <row r="53" spans="1:12" hidden="1">
       <c r="A53" s="3" t="s">
         <v>118</v>
       </c>
@@ -2819,50 +2898,50 @@
       <c r="I53" s="1" t="s">
         <v>132</v>
       </c>
-      <c r="J53" s="11" t="s">
+      <c r="J53" s="10" t="s">
         <v>140</v>
       </c>
     </row>
-    <row r="54" spans="1:10" hidden="1">
-      <c r="A54" s="28"/>
-      <c r="B54" s="29"/>
-      <c r="C54" s="29"/>
-      <c r="D54" s="29"/>
-      <c r="E54" s="29"/>
-      <c r="F54" s="29"/>
-      <c r="G54" s="29"/>
-      <c r="H54" s="29"/>
-      <c r="I54" s="29"/>
-      <c r="J54" s="29"/>
-    </row>
-    <row r="55" spans="1:10" hidden="1">
+    <row r="54" spans="1:12" hidden="1">
+      <c r="A54" s="26"/>
+      <c r="B54" s="27"/>
+      <c r="C54" s="27"/>
+      <c r="D54" s="27"/>
+      <c r="E54" s="27"/>
+      <c r="F54" s="27"/>
+      <c r="G54" s="27"/>
+      <c r="H54" s="27"/>
+      <c r="I54" s="27"/>
+      <c r="J54" s="27"/>
+    </row>
+    <row r="55" spans="1:12" hidden="1">
       <c r="A55" s="1"/>
     </row>
-    <row r="56" spans="1:10" hidden="1">
+    <row r="56" spans="1:12" hidden="1">
       <c r="A56" s="1"/>
     </row>
-    <row r="57" spans="1:10" hidden="1">
+    <row r="57" spans="1:12" hidden="1">
       <c r="A57" s="1"/>
     </row>
-    <row r="58" spans="1:10" hidden="1">
+    <row r="58" spans="1:12" hidden="1">
       <c r="A58" s="1"/>
     </row>
-    <row r="59" spans="1:10" hidden="1">
+    <row r="59" spans="1:12" hidden="1">
       <c r="A59" s="1"/>
     </row>
-    <row r="60" spans="1:10" hidden="1">
+    <row r="60" spans="1:12" hidden="1">
       <c r="A60" s="1"/>
     </row>
-    <row r="61" spans="1:10" hidden="1">
+    <row r="61" spans="1:12" hidden="1">
       <c r="A61" s="1"/>
     </row>
-    <row r="62" spans="1:10" hidden="1">
+    <row r="62" spans="1:12" hidden="1">
       <c r="A62" s="1"/>
     </row>
-    <row r="63" spans="1:10" hidden="1">
+    <row r="63" spans="1:12" hidden="1">
       <c r="A63" s="1"/>
     </row>
-    <row r="64" spans="1:10" hidden="1">
+    <row r="64" spans="1:12" hidden="1">
       <c r="A64" s="1"/>
     </row>
     <row r="65" spans="1:1" hidden="1">
@@ -2884,7 +2963,7 @@
   <autoFilter ref="A1:K69">
     <filterColumn colId="9">
       <filters>
-        <filter val="1. Dados basicos e pessoais"/>
+        <filter val="Instituicao de Ensino x Pandemia"/>
       </filters>
     </filterColumn>
   </autoFilter>
@@ -2926,7 +3005,7 @@
       <c r="A4" t="s">
         <v>147</v>
       </c>
-      <c r="B4" s="30">
+      <c r="B4" s="28">
         <v>0.46</v>
       </c>
     </row>
@@ -2934,7 +3013,7 @@
       <c r="A5" t="s">
         <v>148</v>
       </c>
-      <c r="B5" s="30">
+      <c r="B5" s="28">
         <v>0.02</v>
       </c>
     </row>
@@ -2942,7 +3021,7 @@
       <c r="A6" t="s">
         <v>149</v>
       </c>
-      <c r="B6" s="30">
+      <c r="B6" s="28">
         <v>0.48</v>
       </c>
     </row>
@@ -2950,7 +3029,7 @@
       <c r="A7" t="s">
         <v>150</v>
       </c>
-      <c r="B7" s="30">
+      <c r="B7" s="28">
         <v>0.04</v>
       </c>
     </row>
@@ -3084,10 +3163,10 @@
       <c r="A3" t="s">
         <v>162</v>
       </c>
-      <c r="B3" s="31">
+      <c r="B3" s="29">
         <v>40</v>
       </c>
-      <c r="C3" s="30">
+      <c r="C3" s="28">
         <v>0.77</v>
       </c>
     </row>
@@ -3095,10 +3174,10 @@
       <c r="A4" t="s">
         <v>163</v>
       </c>
-      <c r="B4" s="31">
-        <v>12</v>
-      </c>
-      <c r="C4" s="30">
+      <c r="B4" s="29">
+        <v>12</v>
+      </c>
+      <c r="C4" s="28">
         <v>0.23</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Codigo, grafico e nuvem de palavras sobre questoes instituicao de ensino.
</commit_message>
<xml_diff>
--- a/documentos/dataset_detalhes.xlsx
+++ b/documentos/dataset_detalhes.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="488" uniqueCount="181">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="491" uniqueCount="183">
   <si>
     <t>Sequencia</t>
   </si>
@@ -566,6 +566,12 @@
   </si>
   <si>
     <t>Maioria Sim, retornou todas as atividades</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Utilizacao de ferramenta online pela instituicao . Maioria oportuna </t>
+  </si>
+  <si>
+    <t>Feito nuvem de palavras tem q ajustar</t>
   </si>
 </sst>
 </file>
@@ -1199,9 +1205,9 @@
   <sheetPr filterMode="1"/>
   <dimension ref="A1:AZ69"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K49" sqref="K49"/>
+      <selection pane="bottomLeft" activeCell="K47" sqref="K47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1749,9 +1755,11 @@
         <v>134</v>
       </c>
       <c r="K16" s="1" t="s">
-        <v>120</v>
-      </c>
-      <c r="L16" s="1"/>
+        <v>9</v>
+      </c>
+      <c r="L16" s="1" t="s">
+        <v>182</v>
+      </c>
       <c r="M16" s="1"/>
       <c r="N16" s="1"/>
       <c r="O16" s="1"/>
@@ -2414,21 +2422,22 @@
       <c r="D37" s="25" t="s">
         <v>15</v>
       </c>
-      <c r="E37" s="25" t="s">
-        <v>12</v>
-      </c>
-      <c r="F37" s="25" t="s">
-        <v>8</v>
-      </c>
-      <c r="G37" s="25"/>
-      <c r="H37" s="25" t="s">
-        <v>13</v>
-      </c>
-      <c r="I37" s="25"/>
-      <c r="J37" s="25" t="s">
+      <c r="E37" s="33" t="s">
+        <v>12</v>
+      </c>
+      <c r="F37" s="33" t="s">
+        <v>8</v>
+      </c>
+      <c r="G37" s="33"/>
+      <c r="H37" s="33" t="s">
+        <v>178</v>
+      </c>
+      <c r="I37" s="33"/>
+      <c r="J37" s="33" t="s">
         <v>134</v>
       </c>
-      <c r="L37" s="25"/>
+      <c r="K37" s="33"/>
+      <c r="L37" s="33"/>
     </row>
     <row r="38" spans="1:12" hidden="1">
       <c r="A38" s="20" t="s">
@@ -2693,7 +2702,12 @@
       <c r="J46" s="25" t="s">
         <v>134</v>
       </c>
-      <c r="L46" s="25"/>
+      <c r="K46" s="25" t="s">
+        <v>9</v>
+      </c>
+      <c r="L46" s="25" t="s">
+        <v>181</v>
+      </c>
     </row>
     <row r="47" spans="1:12">
       <c r="A47" s="23" t="s">

</xml_diff>

<commit_message>
Grafcicos e codigo, pandemia
</commit_message>
<xml_diff>
--- a/documentos/dataset_detalhes.xlsx
+++ b/documentos/dataset_detalhes.xlsx
@@ -14,6 +14,7 @@
     <sheet name="1.Sit_emprego" sheetId="5" r:id="rId5"/>
     <sheet name="1.Estado_resid" sheetId="6" r:id="rId6"/>
     <sheet name="1.Inst_ensino" sheetId="7" r:id="rId7"/>
+    <sheet name="Plan1" sheetId="8" r:id="rId8"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Questionario!$A$1:$K$69</definedName>
@@ -23,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="491" uniqueCount="183">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="496" uniqueCount="187">
   <si>
     <t>Sequencia</t>
   </si>
@@ -572,6 +573,18 @@
   </si>
   <si>
     <t>Feito nuvem de palavras tem q ajustar</t>
+  </si>
+  <si>
+    <t>Perfil dos respondentes : Idade de 17 a 24 anos, solteiros, proporcao dividida entre Masculino e Feminino, maioria de SP, maioria empregados no mercado de trabalho, estudantes universidade Publica -  Unesp Bauru cursando PPGMit (maioria na pos Mestrado e Doutorado), não são estudantes nativos porem moram na mesma cidade do Campus em moradia permanente.</t>
+  </si>
+  <si>
+    <t>Perfil Instiuicao na Pandemia : maioria migrou pra virtual, acesso a infra estrutura pioraram, atualmente maioria já voltou a normalidade e os respondentes acharam oportuna as decisoes das instituicoes na pandemia.</t>
+  </si>
+  <si>
+    <t>Maioria não convive com idosos e nem com pessoas com comorbidades</t>
+  </si>
+  <si>
+    <t>Maioria já conviveu com pessoas na quarentena</t>
   </si>
 </sst>
 </file>
@@ -1206,8 +1219,8 @@
   <dimension ref="A1:AZ69"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K47" sqref="K47"/>
+      <pane ySplit="1" topLeftCell="A21" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="K23" sqref="K23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1220,7 +1233,7 @@
     <col min="8" max="8" width="21" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="15" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="30.7109375" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="20.7109375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="65.5703125" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="63.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1316,6 +1329,9 @@
       <c r="L3" s="9" t="s">
         <v>156</v>
       </c>
+      <c r="N3" s="9" t="s">
+        <v>183</v>
+      </c>
     </row>
     <row r="4" spans="1:52" hidden="1">
       <c r="A4" s="7" t="s">
@@ -1657,7 +1673,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="14" spans="1:52">
+    <row r="14" spans="1:52" hidden="1">
       <c r="A14" s="23" t="s">
         <v>79</v>
       </c>
@@ -1690,8 +1706,11 @@
       <c r="L14" s="25" t="s">
         <v>176</v>
       </c>
-    </row>
-    <row r="15" spans="1:52">
+      <c r="M14" s="24" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="15" spans="1:52" hidden="1">
       <c r="A15" s="23" t="s">
         <v>80</v>
       </c>
@@ -1725,7 +1744,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="16" spans="1:52">
+    <row r="16" spans="1:52" hidden="1">
       <c r="A16" s="23" t="s">
         <v>81</v>
       </c>
@@ -1801,7 +1820,7 @@
       <c r="AY16" s="1"/>
       <c r="AZ16" s="1"/>
     </row>
-    <row r="17" spans="1:12">
+    <row r="17" spans="1:12" hidden="1">
       <c r="A17" s="31" t="s">
         <v>82</v>
       </c>
@@ -1933,7 +1952,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="21" spans="1:12" hidden="1">
+    <row r="21" spans="1:12">
       <c r="A21" s="20" t="s">
         <v>86</v>
       </c>
@@ -1956,13 +1975,18 @@
       <c r="H21" s="22" t="s">
         <v>13</v>
       </c>
-      <c r="I21" s="22"/>
+      <c r="I21" s="22" t="s">
+        <v>9</v>
+      </c>
       <c r="J21" s="22" t="s">
         <v>135</v>
       </c>
+      <c r="K21" s="22" t="s">
+        <v>185</v>
+      </c>
       <c r="L21" s="25"/>
     </row>
-    <row r="22" spans="1:12" hidden="1">
+    <row r="22" spans="1:12">
       <c r="A22" s="20" t="s">
         <v>87</v>
       </c>
@@ -1989,9 +2013,12 @@
       <c r="J22" s="22" t="s">
         <v>135</v>
       </c>
+      <c r="K22" s="22" t="s">
+        <v>186</v>
+      </c>
       <c r="L22" s="25"/>
     </row>
-    <row r="23" spans="1:12" hidden="1">
+    <row r="23" spans="1:12">
       <c r="A23" s="20" t="s">
         <v>88</v>
       </c>
@@ -2020,7 +2047,7 @@
       </c>
       <c r="L23" s="25"/>
     </row>
-    <row r="24" spans="1:12" hidden="1">
+    <row r="24" spans="1:12">
       <c r="A24" s="20" t="s">
         <v>89</v>
       </c>
@@ -2049,7 +2076,7 @@
       </c>
       <c r="L24" s="25"/>
     </row>
-    <row r="25" spans="1:12" hidden="1">
+    <row r="25" spans="1:12">
       <c r="A25" s="20" t="s">
         <v>90</v>
       </c>
@@ -2136,7 +2163,7 @@
       </c>
       <c r="L27" s="25"/>
     </row>
-    <row r="28" spans="1:12" hidden="1">
+    <row r="28" spans="1:12">
       <c r="A28" s="20" t="s">
         <v>93</v>
       </c>
@@ -2165,7 +2192,7 @@
       </c>
       <c r="L28" s="25"/>
     </row>
-    <row r="29" spans="1:12" hidden="1">
+    <row r="29" spans="1:12">
       <c r="A29" s="20" t="s">
         <v>94</v>
       </c>
@@ -2254,7 +2281,7 @@
       </c>
       <c r="L31" s="25"/>
     </row>
-    <row r="32" spans="1:12">
+    <row r="32" spans="1:12" hidden="1">
       <c r="A32" s="23" t="s">
         <v>97</v>
       </c>
@@ -2375,7 +2402,7 @@
       </c>
       <c r="L35" s="25"/>
     </row>
-    <row r="36" spans="1:12">
+    <row r="36" spans="1:12" hidden="1">
       <c r="A36" s="23" t="s">
         <v>101</v>
       </c>
@@ -2409,7 +2436,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="37" spans="1:12">
+    <row r="37" spans="1:12" hidden="1">
       <c r="A37" s="23" t="s">
         <v>102</v>
       </c>
@@ -2675,7 +2702,7 @@
       </c>
       <c r="L45" s="25"/>
     </row>
-    <row r="46" spans="1:12">
+    <row r="46" spans="1:12" hidden="1">
       <c r="A46" s="23" t="s">
         <v>111</v>
       </c>
@@ -2709,7 +2736,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="47" spans="1:12">
+    <row r="47" spans="1:12" hidden="1">
       <c r="A47" s="23" t="s">
         <v>112</v>
       </c>
@@ -2740,7 +2767,7 @@
       </c>
       <c r="L47" s="25"/>
     </row>
-    <row r="48" spans="1:12">
+    <row r="48" spans="1:12" hidden="1">
       <c r="A48" s="23" t="s">
         <v>113</v>
       </c>
@@ -2771,7 +2798,7 @@
       </c>
       <c r="L48" s="25"/>
     </row>
-    <row r="49" spans="1:12">
+    <row r="49" spans="1:12" hidden="1">
       <c r="A49" s="23" t="s">
         <v>114</v>
       </c>
@@ -2802,7 +2829,7 @@
       </c>
       <c r="L49" s="25"/>
     </row>
-    <row r="50" spans="1:12" hidden="1">
+    <row r="50" spans="1:12">
       <c r="A50" s="20" t="s">
         <v>115</v>
       </c>
@@ -2830,7 +2857,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="51" spans="1:12" hidden="1">
+    <row r="51" spans="1:12">
       <c r="A51" s="20" t="s">
         <v>116</v>
       </c>
@@ -2858,7 +2885,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="52" spans="1:12" hidden="1">
+    <row r="52" spans="1:12">
       <c r="A52" s="20" t="s">
         <v>117</v>
       </c>
@@ -2977,7 +3004,7 @@
   <autoFilter ref="A1:K69">
     <filterColumn colId="9">
       <filters>
-        <filter val="Instituicao de Ensino x Pandemia"/>
+        <filter val="Pessoa x Pandemia"/>
       </filters>
     </filterColumn>
   </autoFilter>
@@ -3199,4 +3226,16 @@
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData/>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Graficos e codigo R
</commit_message>
<xml_diff>
--- a/documentos/dataset_detalhes.xlsx
+++ b/documentos/dataset_detalhes.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="519" uniqueCount="199">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="525" uniqueCount="202">
   <si>
     <t>Sequencia</t>
   </si>
@@ -621,6 +621,15 @@
   </si>
   <si>
     <t>Todos Vacinados com pelo menos 2 doses</t>
+  </si>
+  <si>
+    <t>Aumentaram ou foram os mesmos na sua maioria</t>
+  </si>
+  <si>
+    <t>Na sua maioria a renda diminuiu ou continou a mesma</t>
+  </si>
+  <si>
+    <t>Maioria não recebeu ajuda financeira da instuicao de ensino ou de outras instituicoes</t>
   </si>
 </sst>
 </file>
@@ -725,7 +734,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="14" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
@@ -781,6 +790,9 @@
     <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1253,8 +1265,8 @@
   <dimension ref="A1:AZ69"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A38" sqref="A38"/>
+      <pane ySplit="1" topLeftCell="A23" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A46" sqref="A46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2637,9 +2649,14 @@
       <c r="H40" s="16" t="s">
         <v>13</v>
       </c>
-      <c r="I40" s="16"/>
+      <c r="I40" s="16" t="s">
+        <v>9</v>
+      </c>
       <c r="J40" s="16" t="s">
         <v>137</v>
+      </c>
+      <c r="K40" s="16" t="s">
+        <v>199</v>
       </c>
       <c r="L40" s="22"/>
     </row>
@@ -2666,38 +2683,48 @@
       <c r="H41" s="16" t="s">
         <v>13</v>
       </c>
-      <c r="I41" s="16"/>
+      <c r="I41" s="16" t="s">
+        <v>9</v>
+      </c>
       <c r="J41" s="16" t="s">
         <v>137</v>
       </c>
+      <c r="K41" s="16" t="s">
+        <v>200</v>
+      </c>
       <c r="L41" s="22"/>
     </row>
     <row r="42" spans="1:12">
-      <c r="A42" s="14" t="s">
+      <c r="A42" s="35" t="s">
         <v>107</v>
       </c>
-      <c r="B42" s="15" t="s">
+      <c r="B42" s="22" t="s">
         <v>55</v>
       </c>
-      <c r="C42" s="16" t="s">
-        <v>123</v>
-      </c>
-      <c r="D42" s="16" t="s">
-        <v>15</v>
-      </c>
-      <c r="E42" s="16" t="s">
+      <c r="C42" s="22" t="s">
+        <v>123</v>
+      </c>
+      <c r="D42" s="22" t="s">
+        <v>15</v>
+      </c>
+      <c r="E42" s="22" t="s">
         <v>12</v>
       </c>
-      <c r="F42" s="16" t="s">
-        <v>8</v>
-      </c>
-      <c r="G42" s="16"/>
-      <c r="H42" s="16" t="s">
+      <c r="F42" s="22" t="s">
+        <v>8</v>
+      </c>
+      <c r="G42" s="22"/>
+      <c r="H42" s="22" t="s">
         <v>13</v>
       </c>
-      <c r="I42" s="16"/>
-      <c r="J42" s="16" t="s">
-        <v>137</v>
+      <c r="I42" s="22" t="s">
+        <v>9</v>
+      </c>
+      <c r="J42" s="22" t="s">
+        <v>134</v>
+      </c>
+      <c r="K42" s="22" t="s">
+        <v>201</v>
       </c>
       <c r="L42" s="22"/>
     </row>
@@ -2813,13 +2840,13 @@
       <c r="H46" s="22" t="s">
         <v>13</v>
       </c>
-      <c r="I46" s="22"/>
+      <c r="I46" s="22" t="s">
+        <v>9</v>
+      </c>
       <c r="J46" s="22" t="s">
         <v>134</v>
       </c>
-      <c r="K46" s="22" t="s">
-        <v>9</v>
-      </c>
+      <c r="K46" s="22"/>
       <c r="L46" s="22" t="s">
         <v>178</v>
       </c>

</xml_diff>

<commit_message>
graficos e codigo (agrupando opcoes)
</commit_message>
<xml_diff>
--- a/documentos/dataset_detalhes.xlsx
+++ b/documentos/dataset_detalhes.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="536" uniqueCount="209">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="540" uniqueCount="213">
   <si>
     <t>Sequencia</t>
   </si>
@@ -650,7 +650,19 @@
     <t>5_Ansiedade_Planejamento.png</t>
   </si>
   <si>
-    <t>5_Ansiedade_Nivel.png</t>
+    <t>5_Ansiedade_Nivel_futuro.png</t>
+  </si>
+  <si>
+    <t>4_Financas_endividamento.png</t>
+  </si>
+  <si>
+    <t>2_Instituicao_ajuda_financeira.png</t>
+  </si>
+  <si>
+    <t>4_Financas_renda.png</t>
+  </si>
+  <si>
+    <t>4_Financas_despesas.png</t>
   </si>
 </sst>
 </file>
@@ -1283,7 +1295,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A32" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K50" sqref="K50"/>
+      <selection pane="bottomLeft" activeCell="K41" sqref="K41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2712,7 +2724,9 @@
       <c r="J40" s="14" t="s">
         <v>137</v>
       </c>
-      <c r="K40" s="14"/>
+      <c r="K40" s="14" t="s">
+        <v>212</v>
+      </c>
       <c r="L40" s="14" t="s">
         <v>199</v>
       </c>
@@ -2747,7 +2761,9 @@
       <c r="J41" s="14" t="s">
         <v>137</v>
       </c>
-      <c r="K41" s="14"/>
+      <c r="K41" s="14" t="s">
+        <v>211</v>
+      </c>
       <c r="L41" s="14" t="s">
         <v>200</v>
       </c>
@@ -2782,7 +2798,9 @@
       <c r="J42" s="20" t="s">
         <v>134</v>
       </c>
-      <c r="K42" s="20"/>
+      <c r="K42" s="20" t="s">
+        <v>210</v>
+      </c>
       <c r="L42" s="20" t="s">
         <v>201</v>
       </c>
@@ -2817,7 +2835,9 @@
       <c r="J43" s="14" t="s">
         <v>137</v>
       </c>
-      <c r="K43" s="14"/>
+      <c r="K43" s="14" t="s">
+        <v>209</v>
+      </c>
       <c r="L43" s="14" t="s">
         <v>202</v>
       </c>

</xml_diff>

<commit_message>
planilha de detalhes do dataset
</commit_message>
<xml_diff>
--- a/documentos/dataset_detalhes.xlsx
+++ b/documentos/dataset_detalhes.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="566" uniqueCount="239">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="569" uniqueCount="242">
   <si>
     <t>Sequencia</t>
   </si>
@@ -741,6 +741,15 @@
   </si>
   <si>
     <t>1_Nome_Cursos.png</t>
+  </si>
+  <si>
+    <t>1_inst_ensino.png</t>
+  </si>
+  <si>
+    <t>1_estado_reside.png</t>
+  </si>
+  <si>
+    <t>1_situacao_empregaticia.png</t>
   </si>
 </sst>
 </file>
@@ -1374,7 +1383,7 @@
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K9" sqref="K9"/>
+      <selection pane="bottomLeft" activeCell="K7" sqref="K7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1589,7 +1598,9 @@
       <c r="J6" s="8" t="s">
         <v>140</v>
       </c>
-      <c r="K6" s="8"/>
+      <c r="K6" s="8" t="s">
+        <v>241</v>
+      </c>
       <c r="L6" s="25" t="s">
         <v>163</v>
       </c>
@@ -1624,7 +1635,9 @@
       <c r="J7" s="8" t="s">
         <v>140</v>
       </c>
-      <c r="K7" s="8"/>
+      <c r="K7" s="8" t="s">
+        <v>240</v>
+      </c>
       <c r="L7" s="8" t="s">
         <v>164</v>
       </c>
@@ -1659,7 +1672,9 @@
       <c r="J8" s="8" t="s">
         <v>140</v>
       </c>
-      <c r="K8" s="8"/>
+      <c r="K8" s="8" t="s">
+        <v>239</v>
+      </c>
       <c r="L8" s="8" t="s">
         <v>156</v>
       </c>

</xml_diff>

<commit_message>
graficos revisados e codigo
</commit_message>
<xml_diff>
--- a/documentos/dataset_detalhes.xlsx
+++ b/documentos/dataset_detalhes.xlsx
@@ -1394,12 +1394,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="1"/>
   <dimension ref="A1:BA69"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K46" sqref="K46"/>
+      <pane ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="K24" sqref="K24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1452,7 +1451,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="2" spans="1:53" hidden="1">
+    <row r="2" spans="1:53">
       <c r="A2" s="3" t="s">
         <v>67</v>
       </c>
@@ -1477,7 +1476,7 @@
       <c r="L2" s="5"/>
       <c r="M2" s="5"/>
     </row>
-    <row r="3" spans="1:53" hidden="1">
+    <row r="3" spans="1:53">
       <c r="A3" s="6" t="s">
         <v>68</v>
       </c>
@@ -1517,7 +1516,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="4" spans="1:53" hidden="1">
+    <row r="4" spans="1:53">
       <c r="A4" s="6" t="s">
         <v>69</v>
       </c>
@@ -1554,7 +1553,7 @@
       </c>
       <c r="M4" s="8"/>
     </row>
-    <row r="5" spans="1:53" hidden="1">
+    <row r="5" spans="1:53">
       <c r="A5" s="6" t="s">
         <v>70</v>
       </c>
@@ -1591,7 +1590,7 @@
       </c>
       <c r="M5" s="8"/>
     </row>
-    <row r="6" spans="1:53" hidden="1">
+    <row r="6" spans="1:53">
       <c r="A6" s="6" t="s">
         <v>71</v>
       </c>
@@ -1628,7 +1627,7 @@
       </c>
       <c r="M6" s="25"/>
     </row>
-    <row r="7" spans="1:53" hidden="1">
+    <row r="7" spans="1:53">
       <c r="A7" s="6" t="s">
         <v>72</v>
       </c>
@@ -1665,7 +1664,7 @@
       </c>
       <c r="M7" s="8"/>
     </row>
-    <row r="8" spans="1:53" hidden="1">
+    <row r="8" spans="1:53">
       <c r="A8" s="6" t="s">
         <v>73</v>
       </c>
@@ -1702,7 +1701,7 @@
       </c>
       <c r="M8" s="8"/>
     </row>
-    <row r="9" spans="1:53" hidden="1">
+    <row r="9" spans="1:53">
       <c r="A9" s="6" t="s">
         <v>74</v>
       </c>
@@ -1739,7 +1738,7 @@
       </c>
       <c r="M9" s="8"/>
     </row>
-    <row r="10" spans="1:53" hidden="1">
+    <row r="10" spans="1:53">
       <c r="A10" s="6" t="s">
         <v>75</v>
       </c>
@@ -1776,7 +1775,7 @@
       </c>
       <c r="M10" s="8"/>
     </row>
-    <row r="11" spans="1:53" hidden="1">
+    <row r="11" spans="1:53">
       <c r="A11" s="3" t="s">
         <v>76</v>
       </c>
@@ -1809,7 +1808,7 @@
       </c>
       <c r="M11" s="5"/>
     </row>
-    <row r="12" spans="1:53" hidden="1">
+    <row r="12" spans="1:53">
       <c r="A12" s="6" t="s">
         <v>77</v>
       </c>
@@ -1846,7 +1845,7 @@
       </c>
       <c r="M12" s="8"/>
     </row>
-    <row r="13" spans="1:53" hidden="1">
+    <row r="13" spans="1:53">
       <c r="A13" s="6" t="s">
         <v>78</v>
       </c>
@@ -2066,7 +2065,7 @@
       <c r="L17" s="5"/>
       <c r="M17" s="5"/>
     </row>
-    <row r="18" spans="1:13" hidden="1">
+    <row r="18" spans="1:13">
       <c r="A18" s="6" t="s">
         <v>83</v>
       </c>
@@ -2102,7 +2101,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="19" spans="1:13" hidden="1">
+    <row r="19" spans="1:13">
       <c r="A19" s="6" t="s">
         <v>84</v>
       </c>
@@ -2138,7 +2137,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="20" spans="1:13" hidden="1">
+    <row r="20" spans="1:13">
       <c r="A20" s="6" t="s">
         <v>85</v>
       </c>
@@ -2174,7 +2173,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="21" spans="1:13" hidden="1">
+    <row r="21" spans="1:13">
       <c r="A21" s="15" t="s">
         <v>86</v>
       </c>
@@ -2203,7 +2202,7 @@
       <c r="J21" s="17" t="s">
         <v>191</v>
       </c>
-      <c r="K21" s="17" t="s">
+      <c r="K21" s="34" t="s">
         <v>226</v>
       </c>
       <c r="L21" s="17" t="s">
@@ -2211,7 +2210,7 @@
       </c>
       <c r="M21" s="22"/>
     </row>
-    <row r="22" spans="1:13" hidden="1">
+    <row r="22" spans="1:13">
       <c r="A22" s="15" t="s">
         <v>87</v>
       </c>
@@ -2240,7 +2239,7 @@
       <c r="J22" s="17" t="s">
         <v>191</v>
       </c>
-      <c r="K22" s="17" t="s">
+      <c r="K22" s="34" t="s">
         <v>225</v>
       </c>
       <c r="L22" s="17" t="s">
@@ -2248,7 +2247,7 @@
       </c>
       <c r="M22" s="22"/>
     </row>
-    <row r="23" spans="1:13" hidden="1">
+    <row r="23" spans="1:13">
       <c r="A23" s="15" t="s">
         <v>88</v>
       </c>
@@ -2277,7 +2276,7 @@
       <c r="J23" s="17" t="s">
         <v>191</v>
       </c>
-      <c r="K23" s="17" t="s">
+      <c r="K23" s="34" t="s">
         <v>224</v>
       </c>
       <c r="L23" s="17" t="s">
@@ -2285,7 +2284,7 @@
       </c>
       <c r="M23" s="22"/>
     </row>
-    <row r="24" spans="1:13" hidden="1">
+    <row r="24" spans="1:13">
       <c r="A24" s="15" t="s">
         <v>89</v>
       </c>
@@ -2314,7 +2313,7 @@
       <c r="J24" s="17" t="s">
         <v>191</v>
       </c>
-      <c r="K24" s="17" t="s">
+      <c r="K24" s="34" t="s">
         <v>223</v>
       </c>
       <c r="L24" s="17" t="s">
@@ -2322,7 +2321,7 @@
       </c>
       <c r="M24" s="22"/>
     </row>
-    <row r="25" spans="1:13" hidden="1">
+    <row r="25" spans="1:13">
       <c r="A25" s="15" t="s">
         <v>90</v>
       </c>
@@ -2359,7 +2358,7 @@
       </c>
       <c r="M25" s="22"/>
     </row>
-    <row r="26" spans="1:13" hidden="1">
+    <row r="26" spans="1:13">
       <c r="A26" s="27" t="s">
         <v>91</v>
       </c>
@@ -2396,7 +2395,7 @@
       </c>
       <c r="M26" s="20"/>
     </row>
-    <row r="27" spans="1:13" hidden="1">
+    <row r="27" spans="1:13">
       <c r="A27" s="26" t="s">
         <v>92</v>
       </c>
@@ -2433,7 +2432,7 @@
       </c>
       <c r="M27" s="20"/>
     </row>
-    <row r="28" spans="1:13" hidden="1">
+    <row r="28" spans="1:13">
       <c r="A28" s="15" t="s">
         <v>93</v>
       </c>
@@ -2470,7 +2469,7 @@
       </c>
       <c r="M28" s="22"/>
     </row>
-    <row r="29" spans="1:13" hidden="1">
+    <row r="29" spans="1:13">
       <c r="A29" s="28" t="s">
         <v>94</v>
       </c>
@@ -2503,7 +2502,7 @@
       <c r="L29" s="30"/>
       <c r="M29" s="30"/>
     </row>
-    <row r="30" spans="1:13" hidden="1">
+    <row r="30" spans="1:13">
       <c r="A30" s="9" t="s">
         <v>95</v>
       </c>
@@ -2540,7 +2539,7 @@
       </c>
       <c r="M30" s="20"/>
     </row>
-    <row r="31" spans="1:13" hidden="1">
+    <row r="31" spans="1:13">
       <c r="A31" s="9" t="s">
         <v>96</v>
       </c>
@@ -2613,7 +2612,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="33" spans="1:13" hidden="1">
+    <row r="33" spans="1:13">
       <c r="A33" s="9" t="s">
         <v>98</v>
       </c>
@@ -2650,7 +2649,7 @@
       </c>
       <c r="M33" s="20"/>
     </row>
-    <row r="34" spans="1:13" hidden="1">
+    <row r="34" spans="1:13">
       <c r="A34" s="9" t="s">
         <v>99</v>
       </c>
@@ -2687,7 +2686,7 @@
       </c>
       <c r="M34" s="20"/>
     </row>
-    <row r="35" spans="1:13" hidden="1">
+    <row r="35" spans="1:13">
       <c r="A35" s="9" t="s">
         <v>100</v>
       </c>
@@ -2791,7 +2790,7 @@
       <c r="L37" s="5"/>
       <c r="M37" s="5"/>
     </row>
-    <row r="38" spans="1:13" hidden="1">
+    <row r="38" spans="1:13">
       <c r="A38" s="32" t="s">
         <v>103</v>
       </c>
@@ -2828,7 +2827,7 @@
       </c>
       <c r="M38" s="20"/>
     </row>
-    <row r="39" spans="1:13" hidden="1">
+    <row r="39" spans="1:13">
       <c r="A39" s="28" t="s">
         <v>104</v>
       </c>
@@ -2861,7 +2860,7 @@
       <c r="L39" s="30"/>
       <c r="M39" s="20"/>
     </row>
-    <row r="40" spans="1:13" hidden="1">
+    <row r="40" spans="1:13">
       <c r="A40" s="12" t="s">
         <v>105</v>
       </c>
@@ -2898,7 +2897,7 @@
       </c>
       <c r="M40" s="20"/>
     </row>
-    <row r="41" spans="1:13" hidden="1">
+    <row r="41" spans="1:13">
       <c r="A41" s="12" t="s">
         <v>106</v>
       </c>
@@ -2972,7 +2971,7 @@
       </c>
       <c r="M42" s="20"/>
     </row>
-    <row r="43" spans="1:13" hidden="1">
+    <row r="43" spans="1:13">
       <c r="A43" s="12" t="s">
         <v>108</v>
       </c>
@@ -3009,7 +3008,7 @@
       </c>
       <c r="M43" s="20"/>
     </row>
-    <row r="44" spans="1:13" hidden="1">
+    <row r="44" spans="1:13">
       <c r="A44" s="28" t="s">
         <v>109</v>
       </c>
@@ -3040,7 +3039,7 @@
       <c r="L44" s="30"/>
       <c r="M44" s="20"/>
     </row>
-    <row r="45" spans="1:13" hidden="1">
+    <row r="45" spans="1:13">
       <c r="A45" s="28" t="s">
         <v>110</v>
       </c>
@@ -3102,7 +3101,7 @@
       <c r="J46" s="20" t="s">
         <v>134</v>
       </c>
-      <c r="K46" s="20" t="s">
+      <c r="K46" s="34" t="s">
         <v>227</v>
       </c>
       <c r="L46" s="20"/>
@@ -3209,7 +3208,7 @@
       <c r="L49" s="30"/>
       <c r="M49" s="20"/>
     </row>
-    <row r="50" spans="1:13" hidden="1">
+    <row r="50" spans="1:13">
       <c r="A50" s="15" t="s">
         <v>115</v>
       </c>
@@ -3245,7 +3244,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="51" spans="1:13" hidden="1">
+    <row r="51" spans="1:13">
       <c r="A51" s="15" t="s">
         <v>116</v>
       </c>
@@ -3281,7 +3280,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="52" spans="1:13" hidden="1">
+    <row r="52" spans="1:13">
       <c r="A52" s="15" t="s">
         <v>117</v>
       </c>
@@ -3317,7 +3316,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="53" spans="1:13" hidden="1">
+    <row r="53" spans="1:13">
       <c r="A53" s="28" t="s">
         <v>118</v>
       </c>
@@ -3349,7 +3348,7 @@
       <c r="K53" s="29"/>
       <c r="L53" s="30"/>
     </row>
-    <row r="54" spans="1:13" hidden="1">
+    <row r="54" spans="1:13">
       <c r="A54" s="21"/>
       <c r="B54" s="22"/>
       <c r="C54" s="22"/>
@@ -3362,58 +3361,54 @@
       <c r="J54" s="22"/>
       <c r="K54" s="22"/>
     </row>
-    <row r="55" spans="1:13" hidden="1">
+    <row r="55" spans="1:13">
       <c r="A55" s="1"/>
     </row>
-    <row r="56" spans="1:13" hidden="1">
+    <row r="56" spans="1:13">
       <c r="A56" s="1"/>
     </row>
-    <row r="57" spans="1:13" hidden="1">
+    <row r="57" spans="1:13">
       <c r="A57" s="1"/>
     </row>
-    <row r="58" spans="1:13" hidden="1">
+    <row r="58" spans="1:13">
       <c r="A58" s="1"/>
     </row>
-    <row r="59" spans="1:13" hidden="1">
+    <row r="59" spans="1:13">
       <c r="A59" s="1"/>
     </row>
-    <row r="60" spans="1:13" hidden="1">
+    <row r="60" spans="1:13">
       <c r="A60" s="1"/>
     </row>
-    <row r="61" spans="1:13" hidden="1">
+    <row r="61" spans="1:13">
       <c r="A61" s="1"/>
     </row>
-    <row r="62" spans="1:13" hidden="1">
+    <row r="62" spans="1:13">
       <c r="A62" s="1"/>
     </row>
-    <row r="63" spans="1:13" hidden="1">
+    <row r="63" spans="1:13">
       <c r="A63" s="1"/>
     </row>
-    <row r="64" spans="1:13" hidden="1">
+    <row r="64" spans="1:13">
       <c r="A64" s="1"/>
     </row>
-    <row r="65" spans="1:1" hidden="1">
+    <row r="65" spans="1:1">
       <c r="A65" s="1"/>
     </row>
-    <row r="66" spans="1:1" hidden="1">
+    <row r="66" spans="1:1">
       <c r="A66" s="1"/>
     </row>
-    <row r="67" spans="1:1" hidden="1">
+    <row r="67" spans="1:1">
       <c r="A67" s="1"/>
     </row>
-    <row r="68" spans="1:1" hidden="1">
+    <row r="68" spans="1:1">
       <c r="A68" s="1"/>
     </row>
-    <row r="69" spans="1:1" hidden="1">
+    <row r="69" spans="1:1">
       <c r="A69" s="1"/>
     </row>
   </sheetData>
   <autoFilter ref="A1:L69">
-    <filterColumn colId="9">
-      <filters>
-        <filter val="Instituicao de Ensino x Pandemia"/>
-      </filters>
-    </filterColumn>
+    <filterColumn colId="9"/>
     <filterColumn colId="10"/>
   </autoFilter>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>

</xml_diff>

<commit_message>
graficos revisados e codigo R
</commit_message>
<xml_diff>
--- a/documentos/dataset_detalhes.xlsx
+++ b/documentos/dataset_detalhes.xlsx
@@ -1398,7 +1398,7 @@
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K25" sqref="K25"/>
+      <selection pane="bottomLeft" activeCell="K31" sqref="K31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2387,7 +2387,7 @@
       <c r="J26" s="17" t="s">
         <v>191</v>
       </c>
-      <c r="K26" s="17" t="s">
+      <c r="K26" s="34" t="s">
         <v>221</v>
       </c>
       <c r="L26" s="17" t="s">
@@ -2424,7 +2424,7 @@
       <c r="J27" s="17" t="s">
         <v>191</v>
       </c>
-      <c r="K27" s="17" t="s">
+      <c r="K27" s="34" t="s">
         <v>220</v>
       </c>
       <c r="L27" s="17" t="s">
@@ -2461,7 +2461,7 @@
       <c r="J28" s="17" t="s">
         <v>191</v>
       </c>
-      <c r="K28" s="17" t="s">
+      <c r="K28" s="34" t="s">
         <v>219</v>
       </c>
       <c r="L28" s="17" t="s">
@@ -2531,7 +2531,7 @@
       <c r="J30" s="11" t="s">
         <v>192</v>
       </c>
-      <c r="K30" s="11" t="s">
+      <c r="K30" s="34" t="s">
         <v>218</v>
       </c>
       <c r="L30" s="17" t="s">
@@ -2568,7 +2568,7 @@
       <c r="J31" s="11" t="s">
         <v>192</v>
       </c>
-      <c r="K31" s="11" t="s">
+      <c r="K31" s="34" t="s">
         <v>217</v>
       </c>
       <c r="L31" s="17" t="s">

</xml_diff>

<commit_message>
planilha e codigo R
</commit_message>
<xml_diff>
--- a/documentos/dataset_detalhes.xlsx
+++ b/documentos/dataset_detalhes.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="572" uniqueCount="245">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="580" uniqueCount="254">
   <si>
     <t>Sequencia</t>
   </si>
@@ -734,9 +734,6 @@
     <t>1_Nome_Cursos.png</t>
   </si>
   <si>
-    <t>1_inst_ensino.png</t>
-  </si>
-  <si>
     <t>1_estado_reside.png</t>
   </si>
   <si>
@@ -746,9 +743,6 @@
     <t>1_Faixas_Etarias.png</t>
   </si>
   <si>
-    <t>1_Genereos.png</t>
-  </si>
-  <si>
     <t>1_Situacao_conjugal.png</t>
   </si>
   <si>
@@ -759,6 +753,39 @@
   </si>
   <si>
     <t>1_Estudante_local_estudo.png</t>
+  </si>
+  <si>
+    <t>1_Generos.png</t>
+  </si>
+  <si>
+    <t>1_instituicao_ensino.png</t>
+  </si>
+  <si>
+    <t>NP1_Situacao_durante_pandemia</t>
+  </si>
+  <si>
+    <t>q</t>
+  </si>
+  <si>
+    <t>NP2_Qualidade_de_vida</t>
+  </si>
+  <si>
+    <t>NP3_Dificuldades_academicas</t>
+  </si>
+  <si>
+    <t>NP4_Dificuldades_financeiras</t>
+  </si>
+  <si>
+    <t>NP5_Instituicao_fez_positivo</t>
+  </si>
+  <si>
+    <t>NP6_Instituicao_poderia_melhorar</t>
+  </si>
+  <si>
+    <t>NP7_instituicao_poderia_ajudar</t>
+  </si>
+  <si>
+    <t>NP8_Detalhes_finais</t>
   </si>
 </sst>
 </file>
@@ -794,7 +821,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="11">
+  <fills count="13">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -855,6 +882,18 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-4.9989318521683403E-2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -869,7 +908,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="41">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="14" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
@@ -927,6 +966,16 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" quotePrefix="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="11" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" quotePrefix="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1397,8 +1446,8 @@
   <dimension ref="A1:BA69"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K31" sqref="K31"/>
+      <pane ySplit="1" topLeftCell="A29" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B44" sqref="B44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1506,7 +1555,7 @@
         <v>140</v>
       </c>
       <c r="K3" s="34" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="L3" s="8" t="s">
         <v>154</v>
@@ -1546,7 +1595,7 @@
         <v>140</v>
       </c>
       <c r="K4" s="34" t="s">
-        <v>240</v>
+        <v>243</v>
       </c>
       <c r="L4" s="8" t="s">
         <v>155</v>
@@ -1583,7 +1632,7 @@
         <v>140</v>
       </c>
       <c r="K5" s="34" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="L5" s="8" t="s">
         <v>162</v>
@@ -1620,7 +1669,7 @@
         <v>140</v>
       </c>
       <c r="K6" s="34" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="L6" s="25" t="s">
         <v>163</v>
@@ -1657,7 +1706,7 @@
         <v>140</v>
       </c>
       <c r="K7" s="34" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="L7" s="8" t="s">
         <v>164</v>
@@ -1694,7 +1743,7 @@
         <v>140</v>
       </c>
       <c r="K8" s="34" t="s">
-        <v>236</v>
+        <v>244</v>
       </c>
       <c r="L8" s="8" t="s">
         <v>156</v>
@@ -1838,7 +1887,7 @@
         <v>140</v>
       </c>
       <c r="K12" s="34" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="L12" s="8" t="s">
         <v>168</v>
@@ -1875,7 +1924,7 @@
         <v>140</v>
       </c>
       <c r="K13" s="34" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="L13" s="8" t="s">
         <v>169</v>
@@ -1960,39 +2009,41 @@
       <c r="M15" s="20"/>
     </row>
     <row r="16" spans="1:53">
-      <c r="A16" s="28" t="s">
+      <c r="A16" s="35" t="s">
         <v>81</v>
       </c>
-      <c r="B16" s="29" t="s">
+      <c r="B16" s="36" t="s">
         <v>29</v>
       </c>
-      <c r="C16" s="29" t="s">
+      <c r="C16" s="36" t="s">
         <v>120</v>
       </c>
-      <c r="D16" s="30" t="s">
-        <v>15</v>
-      </c>
-      <c r="E16" s="29" t="s">
-        <v>8</v>
-      </c>
-      <c r="F16" s="29" t="s">
-        <v>8</v>
-      </c>
-      <c r="G16" s="29"/>
-      <c r="H16" s="29" t="s">
+      <c r="D16" s="37" t="s">
+        <v>15</v>
+      </c>
+      <c r="E16" s="36" t="s">
+        <v>8</v>
+      </c>
+      <c r="F16" s="36" t="s">
+        <v>8</v>
+      </c>
+      <c r="G16" s="36"/>
+      <c r="H16" s="36" t="s">
         <v>18</v>
       </c>
-      <c r="I16" s="29" t="s">
+      <c r="I16" s="36" t="s">
         <v>132</v>
       </c>
-      <c r="J16" s="30" t="s">
+      <c r="J16" s="37" t="s">
         <v>134</v>
       </c>
-      <c r="K16" s="30"/>
-      <c r="L16" s="29" t="s">
+      <c r="K16" s="37" t="s">
+        <v>245</v>
+      </c>
+      <c r="L16" s="36" t="s">
         <v>179</v>
       </c>
-      <c r="M16" s="29"/>
+      <c r="M16" s="36"/>
       <c r="N16" s="1"/>
       <c r="O16" s="1"/>
       <c r="P16" s="1"/>
@@ -2095,7 +2146,7 @@
         <v>140</v>
       </c>
       <c r="K18" s="34" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="L18" s="8" t="s">
         <v>170</v>
@@ -2470,37 +2521,39 @@
       <c r="M28" s="22"/>
     </row>
     <row r="29" spans="1:13">
-      <c r="A29" s="28" t="s">
+      <c r="A29" s="35" t="s">
         <v>94</v>
       </c>
-      <c r="B29" s="29" t="s">
+      <c r="B29" s="36" t="s">
         <v>42</v>
       </c>
-      <c r="C29" s="29" t="s">
+      <c r="C29" s="36" t="s">
         <v>120</v>
       </c>
-      <c r="D29" s="30" t="s">
-        <v>15</v>
-      </c>
-      <c r="E29" s="29" t="s">
-        <v>8</v>
-      </c>
-      <c r="F29" s="29" t="s">
-        <v>8</v>
-      </c>
-      <c r="G29" s="29"/>
-      <c r="H29" s="29" t="s">
+      <c r="D29" s="37" t="s">
+        <v>15</v>
+      </c>
+      <c r="E29" s="36" t="s">
+        <v>8</v>
+      </c>
+      <c r="F29" s="36" t="s">
+        <v>8</v>
+      </c>
+      <c r="G29" s="36"/>
+      <c r="H29" s="36" t="s">
         <v>18</v>
       </c>
-      <c r="I29" s="29" t="s">
+      <c r="I29" s="36" t="s">
         <v>132</v>
       </c>
-      <c r="J29" s="30" t="s">
-        <v>135</v>
-      </c>
-      <c r="K29" s="30"/>
-      <c r="L29" s="30"/>
-      <c r="M29" s="30"/>
+      <c r="J29" s="37" t="s">
+        <v>246</v>
+      </c>
+      <c r="K29" s="37" t="s">
+        <v>247</v>
+      </c>
+      <c r="L29" s="37"/>
+      <c r="M29" s="22"/>
     </row>
     <row r="30" spans="1:13">
       <c r="A30" s="9" t="s">
@@ -2641,7 +2694,7 @@
       <c r="J33" s="11" t="s">
         <v>192</v>
       </c>
-      <c r="K33" s="11" t="s">
+      <c r="K33" s="34" t="s">
         <v>216</v>
       </c>
       <c r="L33" s="17" t="s">
@@ -2678,7 +2731,7 @@
       <c r="J34" s="11" t="s">
         <v>192</v>
       </c>
-      <c r="K34" s="11" t="s">
+      <c r="K34" s="34" t="s">
         <v>215</v>
       </c>
       <c r="L34" s="17" t="s">
@@ -2715,7 +2768,7 @@
       <c r="J35" s="11" t="s">
         <v>192</v>
       </c>
-      <c r="K35" s="11" t="s">
+      <c r="K35" s="34" t="s">
         <v>214</v>
       </c>
       <c r="L35" s="17" t="s">
@@ -2819,7 +2872,7 @@
       <c r="J38" s="8" t="s">
         <v>140</v>
       </c>
-      <c r="K38" s="8" t="s">
+      <c r="K38" s="34" t="s">
         <v>213</v>
       </c>
       <c r="L38" s="8" t="s">
@@ -2828,36 +2881,38 @@
       <c r="M38" s="20"/>
     </row>
     <row r="39" spans="1:13">
-      <c r="A39" s="28" t="s">
+      <c r="A39" s="35" t="s">
         <v>104</v>
       </c>
-      <c r="B39" s="29" t="s">
+      <c r="B39" s="36" t="s">
         <v>52</v>
       </c>
-      <c r="C39" s="29" t="s">
+      <c r="C39" s="36" t="s">
         <v>120</v>
       </c>
-      <c r="D39" s="30" t="s">
-        <v>15</v>
-      </c>
-      <c r="E39" s="29" t="s">
-        <v>8</v>
-      </c>
-      <c r="F39" s="29" t="s">
-        <v>8</v>
-      </c>
-      <c r="G39" s="29"/>
-      <c r="H39" s="29" t="s">
+      <c r="D39" s="37" t="s">
+        <v>15</v>
+      </c>
+      <c r="E39" s="36" t="s">
+        <v>8</v>
+      </c>
+      <c r="F39" s="36" t="s">
+        <v>8</v>
+      </c>
+      <c r="G39" s="36"/>
+      <c r="H39" s="36" t="s">
         <v>18</v>
       </c>
-      <c r="I39" s="29" t="s">
+      <c r="I39" s="36" t="s">
         <v>132</v>
       </c>
-      <c r="J39" s="30" t="s">
+      <c r="J39" s="37" t="s">
         <v>136</v>
       </c>
-      <c r="K39" s="30"/>
-      <c r="L39" s="30"/>
+      <c r="K39" s="38" t="s">
+        <v>248</v>
+      </c>
+      <c r="L39" s="37"/>
       <c r="M39" s="20"/>
     </row>
     <row r="40" spans="1:13">
@@ -2889,7 +2944,7 @@
       <c r="J40" s="14" t="s">
         <v>137</v>
       </c>
-      <c r="K40" s="14" t="s">
+      <c r="K40" s="34" t="s">
         <v>212</v>
       </c>
       <c r="L40" s="14" t="s">
@@ -2926,7 +2981,7 @@
       <c r="J41" s="14" t="s">
         <v>137</v>
       </c>
-      <c r="K41" s="14" t="s">
+      <c r="K41" s="34" t="s">
         <v>211</v>
       </c>
       <c r="L41" s="14" t="s">
@@ -3000,7 +3055,7 @@
       <c r="J43" s="14" t="s">
         <v>137</v>
       </c>
-      <c r="K43" s="14" t="s">
+      <c r="K43" s="34" t="s">
         <v>209</v>
       </c>
       <c r="L43" s="14" t="s">
@@ -3040,37 +3095,39 @@
       <c r="M44" s="20"/>
     </row>
     <row r="45" spans="1:13">
-      <c r="A45" s="28" t="s">
+      <c r="A45" s="39" t="s">
         <v>110</v>
       </c>
-      <c r="B45" s="29" t="s">
+      <c r="B45" s="40" t="s">
         <v>58</v>
       </c>
-      <c r="C45" s="29" t="s">
+      <c r="C45" s="40" t="s">
         <v>120</v>
       </c>
-      <c r="D45" s="30" t="s">
-        <v>15</v>
-      </c>
-      <c r="E45" s="29" t="s">
-        <v>8</v>
-      </c>
-      <c r="F45" s="29" t="s">
-        <v>8</v>
-      </c>
-      <c r="G45" s="29"/>
-      <c r="H45" s="29" t="s">
+      <c r="D45" s="38" t="s">
+        <v>15</v>
+      </c>
+      <c r="E45" s="40" t="s">
+        <v>8</v>
+      </c>
+      <c r="F45" s="40" t="s">
+        <v>8</v>
+      </c>
+      <c r="G45" s="40"/>
+      <c r="H45" s="40" t="s">
         <v>18</v>
       </c>
-      <c r="I45" s="29" t="s">
+      <c r="I45" s="40" t="s">
         <v>132</v>
       </c>
-      <c r="J45" s="30" t="s">
+      <c r="J45" s="38" t="s">
         <v>137</v>
       </c>
-      <c r="K45" s="30"/>
-      <c r="L45" s="30"/>
-      <c r="M45" s="20"/>
+      <c r="K45" s="38" t="s">
+        <v>249</v>
+      </c>
+      <c r="L45" s="38"/>
+      <c r="M45" s="38"/>
     </row>
     <row r="46" spans="1:13">
       <c r="A46" s="18" t="s">
@@ -3110,103 +3167,109 @@
       </c>
     </row>
     <row r="47" spans="1:13">
-      <c r="A47" s="28" t="s">
+      <c r="A47" s="39" t="s">
         <v>112</v>
       </c>
-      <c r="B47" s="29" t="s">
+      <c r="B47" s="40" t="s">
         <v>60</v>
       </c>
-      <c r="C47" s="29" t="s">
+      <c r="C47" s="40" t="s">
         <v>120</v>
       </c>
-      <c r="D47" s="30" t="s">
-        <v>15</v>
-      </c>
-      <c r="E47" s="29" t="s">
-        <v>8</v>
-      </c>
-      <c r="F47" s="29" t="s">
-        <v>8</v>
-      </c>
-      <c r="G47" s="29"/>
-      <c r="H47" s="29" t="s">
+      <c r="D47" s="38" t="s">
+        <v>15</v>
+      </c>
+      <c r="E47" s="40" t="s">
+        <v>8</v>
+      </c>
+      <c r="F47" s="40" t="s">
+        <v>8</v>
+      </c>
+      <c r="G47" s="40"/>
+      <c r="H47" s="40" t="s">
         <v>18</v>
       </c>
-      <c r="I47" s="29" t="s">
+      <c r="I47" s="40" t="s">
         <v>132</v>
       </c>
-      <c r="J47" s="30" t="s">
+      <c r="J47" s="38" t="s">
         <v>134</v>
       </c>
-      <c r="K47" s="30"/>
-      <c r="L47" s="30"/>
-      <c r="M47" s="20"/>
+      <c r="K47" s="38" t="s">
+        <v>250</v>
+      </c>
+      <c r="L47" s="38"/>
+      <c r="M47" s="38"/>
     </row>
     <row r="48" spans="1:13">
-      <c r="A48" s="28" t="s">
+      <c r="A48" s="39" t="s">
         <v>113</v>
       </c>
-      <c r="B48" s="29" t="s">
+      <c r="B48" s="40" t="s">
         <v>61</v>
       </c>
-      <c r="C48" s="29" t="s">
+      <c r="C48" s="40" t="s">
         <v>120</v>
       </c>
-      <c r="D48" s="30" t="s">
-        <v>15</v>
-      </c>
-      <c r="E48" s="29" t="s">
-        <v>8</v>
-      </c>
-      <c r="F48" s="29" t="s">
-        <v>8</v>
-      </c>
-      <c r="G48" s="29"/>
-      <c r="H48" s="29" t="s">
+      <c r="D48" s="38" t="s">
+        <v>15</v>
+      </c>
+      <c r="E48" s="40" t="s">
+        <v>8</v>
+      </c>
+      <c r="F48" s="40" t="s">
+        <v>8</v>
+      </c>
+      <c r="G48" s="40"/>
+      <c r="H48" s="40" t="s">
         <v>18</v>
       </c>
-      <c r="I48" s="29" t="s">
+      <c r="I48" s="40" t="s">
         <v>132</v>
       </c>
-      <c r="J48" s="30" t="s">
+      <c r="J48" s="38" t="s">
         <v>134</v>
       </c>
-      <c r="K48" s="30"/>
-      <c r="L48" s="30"/>
-      <c r="M48" s="20"/>
+      <c r="K48" s="38" t="s">
+        <v>251</v>
+      </c>
+      <c r="L48" s="38"/>
+      <c r="M48" s="38"/>
     </row>
     <row r="49" spans="1:13">
-      <c r="A49" s="28" t="s">
+      <c r="A49" s="39" t="s">
         <v>114</v>
       </c>
-      <c r="B49" s="29" t="s">
+      <c r="B49" s="40" t="s">
         <v>62</v>
       </c>
-      <c r="C49" s="29" t="s">
+      <c r="C49" s="40" t="s">
         <v>120</v>
       </c>
-      <c r="D49" s="30" t="s">
-        <v>15</v>
-      </c>
-      <c r="E49" s="29" t="s">
-        <v>8</v>
-      </c>
-      <c r="F49" s="29" t="s">
-        <v>8</v>
-      </c>
-      <c r="G49" s="29"/>
-      <c r="H49" s="29" t="s">
+      <c r="D49" s="38" t="s">
+        <v>15</v>
+      </c>
+      <c r="E49" s="40" t="s">
+        <v>8</v>
+      </c>
+      <c r="F49" s="40" t="s">
+        <v>8</v>
+      </c>
+      <c r="G49" s="40"/>
+      <c r="H49" s="40" t="s">
         <v>18</v>
       </c>
-      <c r="I49" s="29" t="s">
+      <c r="I49" s="40" t="s">
         <v>132</v>
       </c>
-      <c r="J49" s="30" t="s">
+      <c r="J49" s="38" t="s">
         <v>134</v>
       </c>
-      <c r="K49" s="30"/>
-      <c r="L49" s="30"/>
-      <c r="M49" s="20"/>
+      <c r="K49" s="38" t="s">
+        <v>252</v>
+      </c>
+      <c r="L49" s="38"/>
+      <c r="M49" s="38"/>
     </row>
     <row r="50" spans="1:13">
       <c r="A50" s="15" t="s">
@@ -3237,7 +3300,7 @@
       <c r="J50" s="17" t="s">
         <v>135</v>
       </c>
-      <c r="K50" s="17" t="s">
+      <c r="K50" s="34" t="s">
         <v>208</v>
       </c>
       <c r="L50" s="17" t="s">
@@ -3273,7 +3336,7 @@
       <c r="J51" s="17" t="s">
         <v>135</v>
       </c>
-      <c r="K51" s="17" t="s">
+      <c r="K51" s="34" t="s">
         <v>207</v>
       </c>
       <c r="L51" s="17" t="s">
@@ -3309,7 +3372,7 @@
       <c r="J52" s="17" t="s">
         <v>135</v>
       </c>
-      <c r="K52" s="17" t="s">
+      <c r="K52" s="34" t="s">
         <v>206</v>
       </c>
       <c r="L52" s="17" t="s">
@@ -3320,33 +3383,35 @@
       <c r="A53" s="28" t="s">
         <v>118</v>
       </c>
-      <c r="B53" s="29" t="s">
+      <c r="B53" s="40" t="s">
         <v>66</v>
       </c>
-      <c r="C53" s="29" t="s">
+      <c r="C53" s="40" t="s">
         <v>120</v>
       </c>
-      <c r="D53" s="30" t="s">
-        <v>15</v>
-      </c>
-      <c r="E53" s="29" t="s">
-        <v>8</v>
-      </c>
-      <c r="F53" s="29" t="s">
-        <v>8</v>
-      </c>
-      <c r="G53" s="29"/>
-      <c r="H53" s="29" t="s">
+      <c r="D53" s="38" t="s">
+        <v>15</v>
+      </c>
+      <c r="E53" s="40" t="s">
+        <v>8</v>
+      </c>
+      <c r="F53" s="40" t="s">
+        <v>8</v>
+      </c>
+      <c r="G53" s="40"/>
+      <c r="H53" s="40" t="s">
         <v>18</v>
       </c>
-      <c r="I53" s="29" t="s">
+      <c r="I53" s="40" t="s">
         <v>132</v>
       </c>
-      <c r="J53" s="29" t="s">
+      <c r="J53" s="40" t="s">
         <v>138</v>
       </c>
-      <c r="K53" s="29"/>
-      <c r="L53" s="30"/>
+      <c r="K53" s="38" t="s">
+        <v>253</v>
+      </c>
+      <c r="L53" s="38"/>
     </row>
     <row r="54" spans="1:13">
       <c r="A54" s="21"/>

</xml_diff>